<commit_message>
all figure pages extracted
</commit_message>
<xml_diff>
--- a/no_extracted_figure_papers.xlsx
+++ b/no_extracted_figure_papers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
+          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sutcliffe &amp; McNamara_2001_OrgSci_Controlling Decision Making Practices in Organizations_Quant.pdf</t>
+          <t>Miner et al_2001_ASQ_Organizational Improvisation and Learning_A Field Study.pdf</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
+          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Miner et al_2001_ASQ_Organizational Improvisation and Learning_A Field Study.pdf</t>
+          <t>Sutcliffe &amp; McNamara_2001_OrgSci_Controlling Decision Making Practices in Organizations_Quant.pdf</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
+          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
+          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -598,7 +598,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Edmondson_2002_OrgSci_The Locan and Variegated Nature of Learning in Organizations.pdf</t>
+          <t>Choroszewicz &amp; Kay_2002_HR_The Use of Mobile Technologies for Work to Family Boundary Permeability.pdf</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -608,7 +608,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Orlikowski_2002_OrgSci_Knowing in Practice.pdf</t>
+          <t>Bottom et al._OrgSci_2002_When Talk is Not Cheap Quant.pdf</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -618,7 +618,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Carlile_2002_OrgSci_A Pragmatic view of Knowledge Boundaries.pdf</t>
+          <t>Maoz, Steinberg, Bar-On &amp; Fakhereldeen_2002_HR_The dialogue between the Self and the Other - a process analysis of Palestinian-Jewish encounters in Israel.pdf</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,101 +628,1921 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
+          <t>Ruderman et al._2002_AMJ_Benefits of Multiple Roles for Managerial Women.pdf</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2010</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Rumens_2010__HR_Workplace friendships between men - gay men's perspectives and experiences.pdf</t>
+          <t>Carlile_2002_OrgSci_A Pragmatic view of Knowledge Boundaries.pdf</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2010</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hardy &amp; Maguire_2010_AMJ_Discourse, Field-Configuring Events and Change in Organizations and Institutional Fields.pdf</t>
+          <t>Orlikowski_2002_OrgSci_Knowing in Practice.pdf</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2010</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Van Den Brink, Benschop &amp; Jansen_2010_OrgStudies_Transparency in Academic Recruitment - a Problematic Tool for Gender Equality.pdf</t>
+          <t>Edmondson_2002_OrgSci_The Locan and Variegated Nature of Learning in Organizations.pdf</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2010</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Nielson, Randall &amp; Christensen_2010_HR_Does training managers enhance the effects of implementing team working.pdf</t>
+          <t>Zilber_2002_AMJ_Institutionalization as an Interplay between Actions Meanings and Actors.pdf</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2010</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
+          <t>Bechky_2003_OrgSci_Sharing Meaning across Occupational Communities.pdf</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2010</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
+          <t>Humphreys_2003_J Management Studies_Dress and Identity  A Turkish Case Study.pdf</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2010</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
+          <t>Sorge &amp; Brussig_2003_OrgSci_Organizational Process, Strategic Content and Socio-Economic Resources.pdf</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2010</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
+          <t>Ailon Souday &amp; Kunda_2003_OrgStudies_The Local Selves of Global Workers.pdf</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2010</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Brooks_2003_OrgSci_Systemic Exchange - Responsibility for Angst.pdf</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Darr &amp; Talmud_2003_OrgStudies_The STructure of Knowledge and Seller-Buyer NEtworks in Markets for Emergent Technologies.pdf</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Piderit_2003_J Management Studies - Breaking Silence  Tactical Choices Women Managers Make in Speaking Up About.pdf</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Hardy_2003_J Management Studies _ Resources  Knowledge and Influence  The Organizational Effects of Interorganizational.pdf</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Guerrier &amp; Adib_2003_HR_Work at leisure and leisure at work - a study of the emotional labour of tour reps.pdf</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical and linguistic moves for a moving display.pdf</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical linguistic moves.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>El-Sawad, Arnold &amp; Cohen_2004_HR_Doublethink the prevalence and function of contradiction in accounts of org life.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Graebner &amp; Eisenhardt_2004_ASQ_The Seller's Side of the Story - Acquisiation as Courtship and Governance as Syndicate.pdf</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Procter &amp; Currie_2004_HR_Target based teamworking - groups work and interdependence in the UK Civil Service.pdf</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Banerjee &amp; Linstead_2004_HR_Masking subversion.pdf</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Maguire, Hardy &amp; Lawrence_2004_AMJ_Institutional Entrepreneurship in Emerging Fields HIV AIDS Treatment Advocacy in Canada.pdf</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Collin-Jacques &amp; Smith_2004_HR_Nursing on the line - Experiences from England and Quebec.pdf</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Hoegl et al_2004_OrgSci_Interteam Coordination Project Commitment and Teamwork.pdf</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Clegg_2004_J Management Studies _ Political Hybrids  Tocquevillean Views on Project Organizations.pdf</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Evans et al._2004_ASQ_Beach Time Bridge Time and Billable Hours.pdf</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Cross &amp; Sproull_2004_OrgSci_More Than an Answer - Information Relationships for Actionable Knowledge.pdf</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Whittle_2005_HR_Preaching and practising flexibility.pdf</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Suddaby &amp; Greenwod_2005_ASQ_Rhetorical Strategies of Legitimacy_Content Analysis.pdf</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>D'Abate_2005_HR_Working hard or hardly working - a study of individuals engaging in personal business ont he job.pdf</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Perkins_2005_J Management Studies _ Ordering Top Pay  Interpreting the Signals.pdf</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Fanelli &amp; Grasselli_2005_OrgSci_Defeating the Minotaur - The construction of CEO Charisma on the US Stock Market.pdf</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Hanlon et al._2005_HR_Knowledge, technology and nursing - the case of NHS Direct.pdf</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Goltz_2005_HR_Women's appeals for equity at American universities.pdf</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Ferlie et al._2005_AMJ_The Nonspread of Innovations The Mediating Role of Professionals.pdf</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Dowd &amp; Kaplan_2005_HR_The career life of academics - boundaried or boundaryless.pdf</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Arndt &amp; Bigelow_2005_ASQ_Professionalizing and Masculanizing a Female Occupation_Archival.pdf</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Pio_2005_HR_Knotted strands - working lives of indian women migrants in New Zealand.pdf</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Mano &amp; Gabriel_2006_HR_Workplace romances in cold and hot organizational climates.pdf</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Hong_2006_J Management Studies_ Transferring Organizational Learning Systems to Japanese Subsidiaries in China.pdf</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Ronel_2006_HR_When good overcomes bad - the impact on volunteers on those they help.pdf</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>O'Donohoe &amp; Turley_2006_HR_Compassion at the counter - Service providers and bereaved consumers.pdf</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Klein et al._2006_ASQ_Dynamic Delegation.pdf</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Buchanan et al._2007_HR_Nobody in charge - distributed change agency in healthcare.pdf</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Raz &amp; Fadlon_2007_OrgStudies_Managerial Culture.pdf</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Vermeulen, Van Den Bosch &amp; Volberda_2007_OrgSci_Complex Incremental Product Innovation in Established Service Firms.pdf</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Schwartz &amp; McCann_2007_HR_Overlapping effects - path dependence and path generation in management and organization in Russia.pdf</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Gilmore &amp; Warren_2007_HR_Emotion online - experiences of teaching in a virtual learning environment.pdf</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>O'Mahoney_2007_J Management Studies_The Diffusion of Management Innovations  The Possibilities and Limitations of.pdf</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Desivilya &amp; Yassour-Borochowitz_2008_OrgSci_The Case of CheckpointWatch - A Study of Organizational Practices in a Women's Human Rights Organization.pdf</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Finn_2008_HR_The Language of Teamwork - Reproducing professional divisions in the operating theatre.pdf</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Cooper_2008_HR_The inequality of security - winners and losers in the risk society.pdf</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Katila et al_2008_ASQ_Swimming with Sharks.pdf</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Margolis &amp; Molinsky_2008_AMJ_Navigating the Bind of Necessary Evils.pdf</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>McCann_2008_J Management Studies_Normalized Intensity  The New Labour Process of Middle Management.pdf</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Thompson &amp; Hassenkamp_2008_HR_The social meaning and function of rituals in healthcare practice.pdf</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Pullen &amp; Simpson_2009_HR_Managing differences in feminized work - men otherness and social practice.pdf</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Santos &amp; Eisenhardt_2009_AMJ_Constructing Markets and Shaping Boundaries.pdf</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Currie, Lockett &amp; Suhomlinova_2009_HR_The institutionalization of distributed leadership.pdf</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Chrobot-Mason, Ruderman, Weber and Ernst_2009_HR_The challenge of leading on unstable ground.pdf</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Malenfant_2009_OrgStudies_Risk, Control and Gender - Reconciling PRoduction and Reproduction in the Risk Society.pdf</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Chen, Yao &amp; Kotha_2009_AMJ_Entrepreneur Passion and Preparedness in Business Plan Presentations.pdf</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Shraga &amp; Shirom_2009_HR_The construct validity of vigor and its antecedents.pdf</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Berg, Grant &amp; Johnson_2010_OrgSci_When Callings Are Calling Crafting Work and Leisure in Pursuit of Unanswered Occupational Callings.pdf</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Detert &amp; Trevino_2010_OrgSci_Speaking Up to Higher-Ups.pdf</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Finn, Currie &amp; Martin_2010_OrgStudies_Team Work in Context - Institutional Mediation in the Public-service Professional Bureaucracy.pdf</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Anteby_2010_ASQ_Markets Morals and Practices of Trade.pdf</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Prasad, Prasad &amp; Mir_2010_HR_One Mirror in Another Managing diversity and the discourse of fashion.pdf</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Clarke_2010_J Management Studies_Revitalizing Entrepreneurship  How Visual Symbols are Used in Entrepreneurial.pdf</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>MacLean &amp; Behnam_2010_AMJ_The Dangers of Decoupling.pdf</t>
         </is>
       </c>
-      <c r="B29" t="n">
+      <c r="B88" t="n">
         <v>2010</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Rumens_2010__HR_Workplace friendships between men - gay men's perspectives and experiences.pdf</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Hardy &amp; Maguire_2010_AMJ_Discourse, Field-Configuring Events and Change in Organizations and Institutional Fields.pdf</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Van Den Brink, Benschop &amp; Jansen_2010_OrgStudies_Transparency in Academic Recruitment - a Problematic Tool for Gender Equality.pdf</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Nielson, Randall &amp; Christensen_2010_HR_Does training managers enhance the effects of implementing team working.pdf</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Fiss_2011_AMJ_Building Better Causal Theories.pdf</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Walsh &amp; Bartuken_2011_AMJ_Cheating the Fates Organizational Foundings in the Wake of Demise.pdf</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Elsesser &amp; Lever_2011_HR_Does gender bias against female leaders persist.pdf</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Lee et al._2011_HR_Entangled strands.pdf</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Matusik &amp; Mickel_2011_HR_Embracing or embattled by converged mobile devices.pdf</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Greckhamer_2011_OrgStudies_Cross-cultural Differences in Compensation Level and Inequality across Occupations.pdf</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Willems et al._2012_HR_Volunteer decisions not to leave - reasons to quit versus functional motivates to stay.pdf</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Currie &amp; White_2012_OrgStudies_Inter-professional Barriers and Knowledge Brokering in an Organizational Context.pdf</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Browning &amp; McNamee_2012_HR_Considering the temporary leader in temporary work arrangements.pdf</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Wright, Nyberg &amp; Grant_2012_OrgStudies_Hippies on the third floor - climage change, narrative identity and the micro-politics of corporate environmentalism.pdf</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Grugulis &amp; Stoyanova_2012_OrgStudies_Social Capital and Networks in Film and TV.pdf</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Crowley_2012_OrgStudies_Control and Dignity in Professional, Manual and Service-Sector Employment.pdf</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Sturges_2012_HR_Crafting a balance between work and home.pdf</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Rowlands &amp; Handy_2012_HR_An addictive environment-New Zealand film production workers subjectie experiences of project-based labour.pdf</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Watson &amp; Watson_2012_HR_Narratives in Society.pdf</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Kenny_2012_OrgStudies_Somoene Big and Important.pdf</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Willis_2012_HR_Witnesses on the periphery.pdf</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Leonardi, Neeley &amp; Gerber_2012_OrgSci_How Managers Use Multiple Media.pdf</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Rennstam_2012_OrgStudies_Object Control a Study of Technologically Dense Knowledge Work.pdf</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>McCann_2012_J Management Studies_Still Blue‐Collar after all these Years  An Ethnography of the Professionalization.pdf</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Mork &amp; Hoholm_2012_HR_Changing practice through boundary organizing.pdf</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Heaphy_2013_OrgSci_Repairing Breaches with Rules Maintaining Institutions.pdf</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Candrian_2013_HR_Taming death and the consequences of discourse.pdf</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Benschop et al._2013_HR_Discourses of ambition, gender and part time work.pdf</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Schneider, Bullinger &amp; Brandl_2013_OrgStudies_Resourcing under Tensions.pdf</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Belhoste &amp; Monin_2013_HR_Constructing Difference in a Cross Cultural Context.pdf</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Ashley &amp; Empson_2013_HR_Differentiation and discrimination.pdf</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Nicholson &amp; Carroll_2013_HR_Identity Undoing and power relations in leadership development.pdf</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Costas_2013_OrgStudies_Problematizing Mobility - a Metaphor of Stickiness, non-places and the kinetic elite.pdf</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Campbell &amp; van Wanrooy_2013_HR_Long working hours and working-time preferences.pdf</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>McPherson &amp; Sauder_2013_ASQ_Logics in Action - Managing Institutional Complexity in Drug Court.pdf</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Darr &amp; Pinch_2013_OrgStudies_Performing Sales.pdf</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Michaud_2013_OrgStudies_Mediating hte Paradox of Organizational Governance Through Numbers.pdf</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Dhalla &amp; Oliver_2013_OrgStudies_Industry Identity in an Oligopolistic Market and Firms' Responses to Institutional Pressures.pdf</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Orr_2014_OrgStudies_Local Government Chief Executive.pdf</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Fayard &amp; Metiu_2014_OrgSci_The Role of Writing in Distributed Collaboration.pdf</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Misangyi &amp; Acharya_2014_AMJ_Substitutes or Complements.pdf</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Raffaelli &amp; Glynn_2014_AMJ_Turkey or Tailored Relational Pluralism Institutional Complexity and the Organizational Adoption of More or Less Customized PRactices.pdf</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>Whitford &amp; Zirpoli_2014_OrgSci_Pragmatism, Practice, and the Boundaries of Organization.pdf</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>Tilcsik_2014_ASQ_Imprint-Environment Fit and Performance.pdf</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Costas &amp; Grey_2014_OrgStudies_The Temporality of Power and the Power of Temporality.pdf</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Meuer_2014_OrgStudies_Archetypes of Inter-firm Relations in the Implementation of Management Innovation.pdf</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>McMurray &amp; Ward_2014_Why Would you do that.pdf</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>huising_2015_ASQ_To Hive or to Hold Producing Professional Authority through Scut Work.pdf</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Hawkins_2015_HR_Ship Shape - Materializing leadership in the British Royal Navy.pdf</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Gilmore &amp; Kenny_2015_HR_Work-worlds colliding - self-reflexivity, power and emotion in organizational ethnogrpahy.pdf</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Di Stefano, King &amp; Verona_2015_AMJ_Sanctioning in the Wild Rational Calculus and Retributive Instincts in Gourmet Cuisine.pdf</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Riach &amp; Warren_2015_HR_Smell organization - Bodies and corporeal porosity in office work.pdf</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>McCann, Hassart &amp; Granter_2015_HR_Casting the lean spell.pdf</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Mair, Mayer &amp; Lutz_2015_OrgStudies_Navigating Institutional Plurality  - Organizational Governance in Hybrid Organizations.pdf</t>
+        </is>
+      </c>
+      <c r="B147" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Alcadipani, Westowood &amp; Rosa_2015_HR_The politics of identity in organizational ethnographis research.pdf</t>
+        </is>
+      </c>
+      <c r="B148" t="n">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Aroles &amp; McLean_2016_OrgSci_Rethinking Stability and Change in the Study of Organizational Routines.pdf</t>
+        </is>
+      </c>
+      <c r="B149" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Farias_2016_OrgStudies_Thats what friends are for.pdf</t>
+        </is>
+      </c>
+      <c r="B150" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Whitford &amp; Zirpoli_2016_OrgStudies_The Network Firm as a Political Coalition.pdf</t>
+        </is>
+      </c>
+      <c r="B151" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Reedy, King &amp; Coupland_2016_OrgStudies_Organizing for Individuation.pdf</t>
+        </is>
+      </c>
+      <c r="B152" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Brannan_2016_HR_Power Corruption and Mis-selling.pdf</t>
+        </is>
+      </c>
+      <c r="B153" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Costas &amp; Karreman_2016_HR_The bored self in knowledge work.pdf</t>
+        </is>
+      </c>
+      <c r="B154" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Weiss &amp; Huault_2016_OrgStudies_Business as Usual in Financial Markets - The creation of incommensurables as institutional maintenance work.pdf</t>
+        </is>
+      </c>
+      <c r="B155" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Heinze &amp; Weber_2016_OrgSci_Toward Organizational Pluralism.pdf</t>
+        </is>
+      </c>
+      <c r="B156" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>Nigam et al._2016_ASQ_Explaining the Selection of Routines for Change during Organizational Search.pdf</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>O'Toole &amp; Grey_2016_HR_Beyond Choice Thick Volunteering and the Case of the Royal National Lifeboat Institution.pdf</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Umney_2016_HR_The Labour Market for Jazz Musicians in Paris and London.pdf</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Mavin &amp; Grandy_2016_HR_A Theory of Abject Appearance.pdf</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Low, Bordia &amp; Bordia_2016_HR_What do Employees want and why.pdf</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Nelson_2016_OrgSci_How to Share a Really Good Secret.pdf</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Bishop &amp; Waring_2016_HR_Becoming Hybrid.pdf</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Fernandez, Marti &amp; Farchi_2016_OrgStudies_Mundane and Everyday Politics for and from the neighbourhood.pdf</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Pecis_2016_HR_Doing and undoing gender in innovation - feminities and masculinities in innovation proess.pdf</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Gist-Mackey_2017_Disembodied Job Search Communicaiton Training.pdf</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Farias_2017_OrgStudies_Money is the root of all evil or is it.pdf</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Radoynovska_2017_OrgStudies_Working within Discretionary boundaries.pdf</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Kornberger et al._2017_OrgStudies_When Bureaucracy Meets the Crowd.pdf</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Katila et al._2017_AMJ_Is There a Doctor in the House.pdf</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Blithe &amp; Wolfe_2017_HR_Work -Life Management in Legal Prostitution.pdf</t>
+        </is>
+      </c>
+      <c r="B171" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Kislov, Hyde &amp; McDonald_2017_OrgStudies_New Game Old Rules - Mechanisms and Consequences of Legitimation in Boundary Spanning Activities.pdf</t>
+        </is>
+      </c>
+      <c r="B172" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Visser_2017_J Management Studies _Prying Eyes  A Dramaturgical Approach to Professional Surveillance.pdf</t>
+        </is>
+      </c>
+      <c r="B173" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>Handy &amp; Rowlands_2017_HR_The Systems Psychodynamics of Gendered Hiring.pdf</t>
+        </is>
+      </c>
+      <c r="B174" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Moisander, Grob &amp; Eraranta_2017_Mechanisms of biopower and neliberal governmentality in precarious work.pdf</t>
+        </is>
+      </c>
+      <c r="B175" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Ybema &amp; Horvers_2017_OrgStudies_Resistance Through Compliance.pdf</t>
+        </is>
+      </c>
+      <c r="B176" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Fayard et al._2017_ASQ_How Nascent Occupations Construct a Mandate.pdf</t>
+        </is>
+      </c>
+      <c r="B177" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Pouthier_2017_OrgStudies_Griping and Joking as identificationRituals and Tools for Engagement in Cross-Boundary Team Meetings.pdf</t>
+        </is>
+      </c>
+      <c r="B178" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Ford et al._2017_OrgStudies_Becoming the Leader - Leadership as a Material Presence.pdf</t>
+        </is>
+      </c>
+      <c r="B179" t="n">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Bechky &amp; Chung_2018_ASQ_Latitude or Latent Control- How Occupational Embeddedness and Control Shape Emergent Coordination.pdf</t>
+        </is>
+      </c>
+      <c r="B180" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Thoren, Agerfalk &amp; Rolandsson_2018_OrgStudies_Voicing the Puppet - Accomodating Unresolved Institutional Tensions in Digital Open Practices.pdf</t>
+        </is>
+      </c>
+      <c r="B181" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Hoffman_2018_HR_Talking into Non Existence.pdf</t>
+        </is>
+      </c>
+      <c r="B182" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Le Theule, Lambert &amp; Morales_2018_OrgStudies_Governing Death.pdf</t>
+        </is>
+      </c>
+      <c r="B183" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Fainshmidt_2018_J Management Studies _When do Dynamic Capabilities Lead to Competitive Advantage  The Importance of.pdf</t>
+        </is>
+      </c>
+      <c r="B184" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Bourgoin &amp; Harvey_2018_HR_Professional image under threat.pdf</t>
+        </is>
+      </c>
+      <c r="B185" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Cruz &amp; Meisenback_2018_HR_Expanding Role Boundary Management Theory.pdf</t>
+        </is>
+      </c>
+      <c r="B186" t="n">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Cohen et al._2019_ASQ_The Role of Accelerator Designs in Mitigating Bounded Rationality in New Ventures.pdf</t>
+        </is>
+      </c>
+      <c r="B187" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Sandholtz, Chung &amp; Waisberg_2019_OrgSci_The Double-Edged Sword of Jurisdictional Entrenchment.pdf</t>
+        </is>
+      </c>
+      <c r="B188" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Vincent &amp; Pagan_2019_HR_Entrepreneurial Agency and Field Relations.pdf</t>
+        </is>
+      </c>
+      <c r="B189" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Hales, Riach &amp; Tyler_2019_OrgStudies_Close encounters - intimate service interactions in lap dancing work.pdf</t>
+        </is>
+      </c>
+      <c r="B190" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Foroughi &amp; Al-Amoudi_2019_OrgStudies_Collective forgetting in a changing organization.pdf</t>
+        </is>
+      </c>
+      <c r="B191" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Walsh, Pazzaglia &amp; Ergene_2019_HR_Loyal after the End.pdf</t>
+        </is>
+      </c>
+      <c r="B192" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Guo_2019_HR_Let Our Emotions Tell the Story.pdf</t>
+        </is>
+      </c>
+      <c r="B193" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Jack, Riach &amp; Bariola_2019_HR_Temporality and Gendered Agecy.pdf</t>
+        </is>
+      </c>
+      <c r="B194" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Demetry_2019_OrgSci_How Organizations Claim Authenticity The Coproduction of Illusions in Underground Restaurants.pdf</t>
+        </is>
+      </c>
+      <c r="B195" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Azambula &amp; Islam_2019_HR_Working at the boundaries.pdf</t>
+        </is>
+      </c>
+      <c r="B196" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Van Hulst &amp; Ybema_2019_From What to Where.pdf</t>
+        </is>
+      </c>
+      <c r="B197" t="n">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Rennstam &amp; Karreman_2020_HR_Understanding control in communities of practice.pdf</t>
+        </is>
+      </c>
+      <c r="B198" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Chliova, Mair &amp; Vernis_2020_OrgStudies_Persistent Category Ambiguity - The case of social entrepreneurship.pdf</t>
+        </is>
+      </c>
+      <c r="B199" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Hallen, Cohen &amp; Bingham_2020_OrgSci_Do Accelerators Work If So, How.pdf</t>
+        </is>
+      </c>
+      <c r="B200" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>DeCelles &amp; Anteby_2020_OrgSci_Compassion in the Clink When and How Human Services Workers Overcome Barriers to Care.pdf</t>
+        </is>
+      </c>
+      <c r="B201" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Skovgaard-Smith, Soekijad &amp; Down_2020_HR_The Other side of us.pdf</t>
+        </is>
+      </c>
+      <c r="B202" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Katila, Kuismin &amp; Valtonen_2020_HR_Becoming upbeat.pdf</t>
+        </is>
+      </c>
+      <c r="B203" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Kenny, Haugh &amp; Fotaki_2020_HR_Organizational Form and Pro-Social Fantasy in Social Enterprise Creation.pdf</t>
+        </is>
+      </c>
+      <c r="B204" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Brown et al._2020_HR_Organizing the Sensory.pdf</t>
+        </is>
+      </c>
+      <c r="B205" t="n">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Garcia-Lorenzo, Sell-Trujillo &amp; Donnelly_2021_OrgStudies_Responding to Stigmatization - how to resist and overcome the stigma of unemployment.pdf</t>
+        </is>
+      </c>
+      <c r="B206" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Dawson &amp; Bencherki_2021_HR_Federal Employees or Rogue Rangers.pdf</t>
+        </is>
+      </c>
+      <c r="B207" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Burchiellaro_2021_OrgStudies_Queering Control and Inclusion the Contemporary Organization.pdf</t>
+        </is>
+      </c>
+      <c r="B208" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Brooks, Grgulis &amp; Cook_2021_HR_Unlearning and consent in the UK Fire and Rescue Service.pdf</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Morlacchi_2021_OrgStudies_The Performative Power of Frictions and New Possibilities.pdf</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Kozhevnikov_2021_HR_Career Capital in Global Vs Second Order Cities.pdf</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new extracted figure pages - corrected file naming
</commit_message>
<xml_diff>
--- a/no_extracted_figure_papers.xlsx
+++ b/no_extracted_figure_papers.xlsx
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
+          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sutcliffe &amp; McNamara_2001_OrgSci_Controlling Decision Making Practices in Organizations_Quant.pdf</t>
+          <t>Miner et al_2001_ASQ_Organizational Improvisation and Learning_A Field Study.pdf</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
+          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Miner et al_2001_ASQ_Organizational Improvisation and Learning_A Field Study.pdf</t>
+          <t>Sutcliffe &amp; McNamara_2001_OrgSci_Controlling Decision Making Practices in Organizations_Quant.pdf</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
+          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
+          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -678,7 +678,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Piderit_2003_J Management Studies - Breaking Silence  Tactical Choices Women Managers Make in Speaking Up About.pdf</t>
+          <t>Sorge &amp; Brussig_2003_OrgSci_Organizational Process, Strategic Content and Socio-Economic Resources.pdf</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -688,7 +688,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Guerrier &amp; Adib_2003_HR_Work at leisure and leisure at work - a study of the emotional labour of tour reps.pdf</t>
+          <t>Brooks_2003_OrgSci_Systemic Exchange - Responsibility for Angst.pdf</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -698,7 +698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Hardy_2003_J Management Studies _ Resources  Knowledge and Influence  The Organizational Effects of Interorganizational.pdf</t>
+          <t>Bechky_2003_OrgSci_Sharing Meaning across Occupational Communities.pdf</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -708,7 +708,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Darr &amp; Talmud_2003_OrgStudies_The STructure of Knowledge and Seller-Buyer NEtworks in Markets for Emergent Technologies.pdf</t>
+          <t>Ailon Souday &amp; Kunda_2003_OrgStudies_The Local Selves of Global Workers.pdf</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -718,7 +718,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Humphreys_2003_J Management Studies_Dress and Identity  A Turkish Case Study.pdf</t>
+          <t>Guerrier &amp; Adib_2003_HR_Work at leisure and leisure at work - a study of the emotional labour of tour reps.pdf</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -728,7 +728,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ailon Souday &amp; Kunda_2003_OrgStudies_The Local Selves of Global Workers.pdf</t>
+          <t>Darr &amp; Talmud_2003_OrgStudies_The STructure of Knowledge and Seller-Buyer NEtworks in Markets for Emergent Technologies.pdf</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -738,7 +738,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Sorge &amp; Brussig_2003_OrgSci_Organizational Process, Strategic Content and Socio-Economic Resources.pdf</t>
+          <t>Hardy_2003_J Management Studies _ Resources  Knowledge and Influence  The Organizational Effects of Interorganizational.pdf</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -748,7 +748,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bechky_2003_OrgSci_Sharing Meaning across Occupational Communities.pdf</t>
+          <t>Piderit_2003_J Management Studies - Breaking Silence  Tactical Choices Women Managers Make in Speaking Up About.pdf</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,7 +758,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Brooks_2003_OrgSci_Systemic Exchange - Responsibility for Angst.pdf</t>
+          <t>Humphreys_2003_J Management Studies_Dress and Identity  A Turkish Case Study.pdf</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -768,7 +768,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cross &amp; Sproull_2004_OrgSci_More Than an Answer - Information Relationships for Actionable Knowledge.pdf</t>
+          <t>Banerjee &amp; Linstead_2004_HR_Masking subversion.pdf</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -778,7 +778,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Evans et al._2004_ASQ_Beach Time Bridge Time and Billable Hours.pdf</t>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical and linguistic moves for a moving display.pdf</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -788,7 +788,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Clegg_2004_J Management Studies _ Political Hybrids  Tocquevillean Views on Project Organizations.pdf</t>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical linguistic moves.pdf</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,7 +798,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Hoegl et al_2004_OrgSci_Interteam Coordination Project Commitment and Teamwork.pdf</t>
+          <t>El-Sawad, Arnold &amp; Cohen_2004_HR_Doublethink the prevalence and function of contradiction in accounts of org life.pdf</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -808,7 +808,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Collin-Jacques &amp; Smith_2004_HR_Nursing on the line - Experiences from England and Quebec.pdf</t>
+          <t>Graebner &amp; Eisenhardt_2004_ASQ_The Seller's Side of the Story - Acquisiation as Courtship and Governance as Syndicate.pdf</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -818,7 +818,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Maguire, Hardy &amp; Lawrence_2004_AMJ_Institutional Entrepreneurship in Emerging Fields HIV AIDS Treatment Advocacy in Canada.pdf</t>
+          <t>Procter &amp; Currie_2004_HR_Target based teamworking - groups work and interdependence in the UK Civil Service.pdf</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -828,7 +828,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Procter &amp; Currie_2004_HR_Target based teamworking - groups work and interdependence in the UK Civil Service.pdf</t>
+          <t>Collin-Jacques &amp; Smith_2004_HR_Nursing on the line - Experiences from England and Quebec.pdf</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -838,7 +838,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Graebner &amp; Eisenhardt_2004_ASQ_The Seller's Side of the Story - Acquisiation as Courtship and Governance as Syndicate.pdf</t>
+          <t>Hoegl et al_2004_OrgSci_Interteam Coordination Project Commitment and Teamwork.pdf</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -848,7 +848,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>El-Sawad, Arnold &amp; Cohen_2004_HR_Doublethink the prevalence and function of contradiction in accounts of org life.pdf</t>
+          <t>Clegg_2004_J Management Studies _ Political Hybrids  Tocquevillean Views on Project Organizations.pdf</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -858,7 +858,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical linguistic moves.pdf</t>
+          <t>Evans et al._2004_ASQ_Beach Time Bridge Time and Billable Hours.pdf</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -868,7 +868,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical and linguistic moves for a moving display.pdf</t>
+          <t>Cross &amp; Sproull_2004_OrgSci_More Than an Answer - Information Relationships for Actionable Knowledge.pdf</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -878,7 +878,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Banerjee &amp; Linstead_2004_HR_Masking subversion.pdf</t>
+          <t>Maguire, Hardy &amp; Lawrence_2004_AMJ_Institutional Entrepreneurship in Emerging Fields HIV AIDS Treatment Advocacy in Canada.pdf</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -888,7 +888,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Goltz_2005_HR_Women's appeals for equity at American universities.pdf</t>
+          <t>Perkins_2005_J Management Studies _ Ordering Top Pay  Interpreting the Signals.pdf</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -898,7 +898,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Arndt &amp; Bigelow_2005_ASQ_Professionalizing and Masculanizing a Female Occupation_Archival.pdf</t>
+          <t>Whittle_2005_HR_Preaching and practising flexibility.pdf</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Dowd &amp; Kaplan_2005_HR_The career life of academics - boundaried or boundaryless.pdf</t>
+          <t>Suddaby &amp; Greenwod_2005_ASQ_Rhetorical Strategies of Legitimacy_Content Analysis.pdf</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,7 +918,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ferlie et al._2005_AMJ_The Nonspread of Innovations The Mediating Role of Professionals.pdf</t>
+          <t>D'Abate_2005_HR_Working hard or hardly working - a study of individuals engaging in personal business ont he job.pdf</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -928,7 +928,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Hanlon et al._2005_HR_Knowledge, technology and nursing - the case of NHS Direct.pdf</t>
+          <t>Pio_2005_HR_Knotted strands - working lives of indian women migrants in New Zealand.pdf</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -938,7 +938,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Pio_2005_HR_Knotted strands - working lives of indian women migrants in New Zealand.pdf</t>
+          <t>Fanelli &amp; Grasselli_2005_OrgSci_Defeating the Minotaur - The construction of CEO Charisma on the US Stock Market.pdf</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Perkins_2005_J Management Studies _ Ordering Top Pay  Interpreting the Signals.pdf</t>
+          <t>Ferlie et al._2005_AMJ_The Nonspread of Innovations The Mediating Role of Professionals.pdf</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,7 +958,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>D'Abate_2005_HR_Working hard or hardly working - a study of individuals engaging in personal business ont he job.pdf</t>
+          <t>Dowd &amp; Kaplan_2005_HR_The career life of academics - boundaried or boundaryless.pdf</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -968,7 +968,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Suddaby &amp; Greenwod_2005_ASQ_Rhetorical Strategies of Legitimacy_Content Analysis.pdf</t>
+          <t>Arndt &amp; Bigelow_2005_ASQ_Professionalizing and Masculanizing a Female Occupation_Archival.pdf</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -978,7 +978,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Whittle_2005_HR_Preaching and practising flexibility.pdf</t>
+          <t>Goltz_2005_HR_Women's appeals for equity at American universities.pdf</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -988,7 +988,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Fanelli &amp; Grasselli_2005_OrgSci_Defeating the Minotaur - The construction of CEO Charisma on the US Stock Market.pdf</t>
+          <t>Hanlon et al._2005_HR_Knowledge, technology and nursing - the case of NHS Direct.pdf</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -1048,7 +1048,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>O'Mahoney_2007_J Management Studies_The Diffusion of Management Innovations  The Possibilities and Limitations of.pdf</t>
+          <t>Buchanan et al._2007_HR_Nobody in charge - distributed change agency in healthcare.pdf</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1058,7 +1058,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Gilmore &amp; Warren_2007_HR_Emotion online - experiences of teaching in a virtual learning environment.pdf</t>
+          <t>Raz &amp; Fadlon_2007_OrgStudies_Managerial Culture.pdf</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1068,7 +1068,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Schwartz &amp; McCann_2007_HR_Overlapping effects - path dependence and path generation in management and organization in Russia.pdf</t>
+          <t>Vermeulen, Van Den Bosch &amp; Volberda_2007_OrgSci_Complex Incremental Product Innovation in Established Service Firms.pdf</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1078,7 +1078,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Vermeulen, Van Den Bosch &amp; Volberda_2007_OrgSci_Complex Incremental Product Innovation in Established Service Firms.pdf</t>
+          <t>Schwartz &amp; McCann_2007_HR_Overlapping effects - path dependence and path generation in management and organization in Russia.pdf</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1088,7 +1088,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Raz &amp; Fadlon_2007_OrgStudies_Managerial Culture.pdf</t>
+          <t>Gilmore &amp; Warren_2007_HR_Emotion online - experiences of teaching in a virtual learning environment.pdf</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -1098,7 +1098,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Buchanan et al._2007_HR_Nobody in charge - distributed change agency in healthcare.pdf</t>
+          <t>O'Mahoney_2007_J Management Studies_The Diffusion of Management Innovations  The Possibilities and Limitations of.pdf</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1178,7 +1178,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Chen, Yao &amp; Kotha_2009_AMJ_Entrepreneur Passion and Preparedness in Business Plan Presentations.pdf</t>
+          <t>Pullen &amp; Simpson_2009_HR_Managing differences in feminized work - men otherness and social practice.pdf</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -1188,7 +1188,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Malenfant_2009_OrgStudies_Risk, Control and Gender - Reconciling PRoduction and Reproduction in the Risk Society.pdf</t>
+          <t>Santos &amp; Eisenhardt_2009_AMJ_Constructing Markets and Shaping Boundaries.pdf</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -1198,7 +1198,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Chrobot-Mason, Ruderman, Weber and Ernst_2009_HR_The challenge of leading on unstable ground.pdf</t>
+          <t>Shraga &amp; Shirom_2009_HR_The construct validity of vigor and its antecedents.pdf</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -1208,7 +1208,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Shraga &amp; Shirom_2009_HR_The construct validity of vigor and its antecedents.pdf</t>
+          <t>Currie, Lockett &amp; Suhomlinova_2009_HR_The institutionalization of distributed leadership.pdf</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -1218,7 +1218,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Santos &amp; Eisenhardt_2009_AMJ_Constructing Markets and Shaping Boundaries.pdf</t>
+          <t>Malenfant_2009_OrgStudies_Risk, Control and Gender - Reconciling PRoduction and Reproduction in the Risk Society.pdf</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -1228,7 +1228,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Pullen &amp; Simpson_2009_HR_Managing differences in feminized work - men otherness and social practice.pdf</t>
+          <t>Chen, Yao &amp; Kotha_2009_AMJ_Entrepreneur Passion and Preparedness in Business Plan Presentations.pdf</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -1238,7 +1238,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Currie, Lockett &amp; Suhomlinova_2009_HR_The institutionalization of distributed leadership.pdf</t>
+          <t>Chrobot-Mason, Ruderman, Weber and Ernst_2009_HR_The challenge of leading on unstable ground.pdf</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -1248,7 +1248,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
+          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1258,7 +1258,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
+          <t>Berg, Grant &amp; Johnson_2010_OrgSci_When Callings Are Calling Crafting Work and Leisure in Pursuit of Unanswered Occupational Callings.pdf</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1268,7 +1268,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
+          <t>Detert &amp; Trevino_2010_OrgSci_Speaking Up to Higher-Ups.pdf</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1278,7 +1278,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Nielson, Randall &amp; Christensen_2010_HR_Does training managers enhance the effects of implementing team working.pdf</t>
+          <t>Anteby_2010_ASQ_Markets Morals and Practices of Trade.pdf</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1288,7 +1288,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Van Den Brink, Benschop &amp; Jansen_2010_OrgStudies_Transparency in Academic Recruitment - a Problematic Tool for Gender Equality.pdf</t>
+          <t>Prasad, Prasad &amp; Mir_2010_HR_One Mirror in Another Managing diversity and the discourse of fashion.pdf</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1298,7 +1298,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Hardy &amp; Maguire_2010_AMJ_Discourse, Field-Configuring Events and Change in Organizations and Institutional Fields.pdf</t>
+          <t>Clarke_2010_J Management Studies_Revitalizing Entrepreneurship  How Visual Symbols are Used in Entrepreneurial.pdf</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1308,7 +1308,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Rumens_2010__HR_Workplace friendships between men - gay men's perspectives and experiences.pdf</t>
+          <t>MacLean &amp; Behnam_2010_AMJ_The Dangers of Decoupling.pdf</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1318,7 +1318,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
+          <t>Finn, Currie &amp; Martin_2010_OrgStudies_Team Work in Context - Institutional Mediation in the Public-service Professional Bureaucracy.pdf</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1328,7 +1328,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MacLean &amp; Behnam_2010_AMJ_The Dangers of Decoupling.pdf</t>
+          <t>Rumens_2010__HR_Workplace friendships between men - gay men's perspectives and experiences.pdf</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -1338,7 +1338,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Clarke_2010_J Management Studies_Revitalizing Entrepreneurship  How Visual Symbols are Used in Entrepreneurial.pdf</t>
+          <t>Hardy &amp; Maguire_2010_AMJ_Discourse, Field-Configuring Events and Change in Organizations and Institutional Fields.pdf</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -1348,7 +1348,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Prasad, Prasad &amp; Mir_2010_HR_One Mirror in Another Managing diversity and the discourse of fashion.pdf</t>
+          <t>Van Den Brink, Benschop &amp; Jansen_2010_OrgStudies_Transparency in Academic Recruitment - a Problematic Tool for Gender Equality.pdf</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -1358,7 +1358,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Anteby_2010_ASQ_Markets Morals and Practices of Trade.pdf</t>
+          <t>Nielson, Randall &amp; Christensen_2010_HR_Does training managers enhance the effects of implementing team working.pdf</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -1368,7 +1368,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Finn, Currie &amp; Martin_2010_OrgStudies_Team Work in Context - Institutional Mediation in the Public-service Professional Bureaucracy.pdf</t>
+          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -1378,7 +1378,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Detert &amp; Trevino_2010_OrgSci_Speaking Up to Higher-Ups.pdf</t>
+          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -1388,7 +1388,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Berg, Grant &amp; Johnson_2010_OrgSci_When Callings Are Calling Crafting Work and Leisure in Pursuit of Unanswered Occupational Callings.pdf</t>
+          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1398,7 +1398,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
+          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -1408,7 +1408,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Greckhamer_2011_OrgStudies_Cross-cultural Differences in Compensation Level and Inequality across Occupations.pdf</t>
+          <t>Walsh &amp; Bartuken_2011_AMJ_Cheating the Fates Organizational Foundings in the Wake of Demise.pdf</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -1418,7 +1418,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Matusik &amp; Mickel_2011_HR_Embracing or embattled by converged mobile devices.pdf</t>
+          <t>Fiss_2011_AMJ_Building Better Causal Theories.pdf</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -1428,7 +1428,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Lee et al._2011_HR_Entangled strands.pdf</t>
+          <t>Elsesser &amp; Lever_2011_HR_Does gender bias against female leaders persist.pdf</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -1438,7 +1438,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Elsesser &amp; Lever_2011_HR_Does gender bias against female leaders persist.pdf</t>
+          <t>Lee et al._2011_HR_Entangled strands.pdf</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -1448,7 +1448,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Fiss_2011_AMJ_Building Better Causal Theories.pdf</t>
+          <t>Greckhamer_2011_OrgStudies_Cross-cultural Differences in Compensation Level and Inequality across Occupations.pdf</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -1458,7 +1458,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Walsh &amp; Bartuken_2011_AMJ_Cheating the Fates Organizational Foundings in the Wake of Demise.pdf</t>
+          <t>Matusik &amp; Mickel_2011_HR_Embracing or embattled by converged mobile devices.pdf</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -1468,7 +1468,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Watson &amp; Watson_2012_HR_Narratives in Society.pdf</t>
+          <t>Crowley_2012_OrgStudies_Control and Dignity in Professional, Manual and Service-Sector Employment.pdf</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -1478,7 +1478,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Mork &amp; Hoholm_2012_HR_Changing practice through boundary organizing.pdf</t>
+          <t>Willems et al._2012_HR_Volunteer decisions not to leave - reasons to quit versus functional motivates to stay.pdf</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -1488,7 +1488,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>McCann_2012_J Management Studies_Still Blue‐Collar after all these Years  An Ethnography of the Professionalization.pdf</t>
+          <t>Currie &amp; White_2012_OrgStudies_Inter-professional Barriers and Knowledge Brokering in an Organizational Context.pdf</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -1498,7 +1498,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Rennstam_2012_OrgStudies_Object Control a Study of Technologically Dense Knowledge Work.pdf</t>
+          <t>Browning &amp; McNamee_2012_HR_Considering the temporary leader in temporary work arrangements.pdf</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1508,7 +1508,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Willis_2012_HR_Witnesses on the periphery.pdf</t>
+          <t>Wright, Nyberg &amp; Grant_2012_OrgStudies_Hippies on the third floor - climage change, narrative identity and the micro-politics of corporate environmentalism.pdf</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -1518,7 +1518,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Kenny_2012_OrgStudies_Somoene Big and Important.pdf</t>
+          <t>Grugulis &amp; Stoyanova_2012_OrgStudies_Social Capital and Networks in Film and TV.pdf</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -1528,7 +1528,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Rowlands &amp; Handy_2012_HR_An addictive environment-New Zealand film production workers subjectie experiences of project-based labour.pdf</t>
+          <t>Leonardi, Neeley &amp; Gerber_2012_OrgSci_How Managers Use Multiple Media.pdf</t>
         </is>
       </c>
       <c r="B110" t="n">
@@ -1538,7 +1538,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Leonardi, Neeley &amp; Gerber_2012_OrgSci_How Managers Use Multiple Media.pdf</t>
+          <t>Sturges_2012_HR_Crafting a balance between work and home.pdf</t>
         </is>
       </c>
       <c r="B111" t="n">
@@ -1548,7 +1548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Crowley_2012_OrgStudies_Control and Dignity in Professional, Manual and Service-Sector Employment.pdf</t>
+          <t>Kenny_2012_OrgStudies_Somoene Big and Important.pdf</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -1558,7 +1558,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Grugulis &amp; Stoyanova_2012_OrgStudies_Social Capital and Networks in Film and TV.pdf</t>
+          <t>Willis_2012_HR_Witnesses on the periphery.pdf</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -1568,7 +1568,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Wright, Nyberg &amp; Grant_2012_OrgStudies_Hippies on the third floor - climage change, narrative identity and the micro-politics of corporate environmentalism.pdf</t>
+          <t>Rennstam_2012_OrgStudies_Object Control a Study of Technologically Dense Knowledge Work.pdf</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -1578,7 +1578,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Sturges_2012_HR_Crafting a balance between work and home.pdf</t>
+          <t>Rowlands &amp; Handy_2012_HR_An addictive environment-New Zealand film production workers subjectie experiences of project-based labour.pdf</t>
         </is>
       </c>
       <c r="B115" t="n">
@@ -1588,7 +1588,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Browning &amp; McNamee_2012_HR_Considering the temporary leader in temporary work arrangements.pdf</t>
+          <t>McCann_2012_J Management Studies_Still Blue‐Collar after all these Years  An Ethnography of the Professionalization.pdf</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -1598,7 +1598,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Currie &amp; White_2012_OrgStudies_Inter-professional Barriers and Knowledge Brokering in an Organizational Context.pdf</t>
+          <t>Mork &amp; Hoholm_2012_HR_Changing practice through boundary organizing.pdf</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -1608,7 +1608,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Willems et al._2012_HR_Volunteer decisions not to leave - reasons to quit versus functional motivates to stay.pdf</t>
+          <t>Watson &amp; Watson_2012_HR_Narratives in Society.pdf</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -1618,7 +1618,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Dhalla &amp; Oliver_2013_OrgStudies_Industry Identity in an Oligopolistic Market and Firms' Responses to Institutional Pressures.pdf</t>
+          <t>Ashley &amp; Empson_2013_HR_Differentiation and discrimination.pdf</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -1628,7 +1628,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Michaud_2013_OrgStudies_Mediating hte Paradox of Organizational Governance Through Numbers.pdf</t>
+          <t>Heaphy_2013_OrgSci_Repairing Breaches with Rules Maintaining Institutions.pdf</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -1638,7 +1638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Darr &amp; Pinch_2013_OrgStudies_Performing Sales.pdf</t>
+          <t>Candrian_2013_HR_Taming death and the consequences of discourse.pdf</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -1648,7 +1648,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Campbell &amp; van Wanrooy_2013_HR_Long working hours and working-time preferences.pdf</t>
+          <t>Schneider, Bullinger &amp; Brandl_2013_OrgStudies_Resourcing under Tensions.pdf</t>
         </is>
       </c>
       <c r="B122" t="n">
@@ -1658,7 +1658,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Costas_2013_OrgStudies_Problematizing Mobility - a Metaphor of Stickiness, non-places and the kinetic elite.pdf</t>
+          <t>Belhoste &amp; Monin_2013_HR_Constructing Difference in a Cross Cultural Context.pdf</t>
         </is>
       </c>
       <c r="B123" t="n">
@@ -1668,7 +1668,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Nicholson &amp; Carroll_2013_HR_Identity Undoing and power relations in leadership development.pdf</t>
+          <t>McPherson &amp; Sauder_2013_ASQ_Logics in Action - Managing Institutional Complexity in Drug Court.pdf</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -1678,7 +1678,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>McPherson &amp; Sauder_2013_ASQ_Logics in Action - Managing Institutional Complexity in Drug Court.pdf</t>
+          <t>Benschop et al._2013_HR_Discourses of ambition, gender and part time work.pdf</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -1688,7 +1688,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Belhoste &amp; Monin_2013_HR_Constructing Difference in a Cross Cultural Context.pdf</t>
+          <t>Costas_2013_OrgStudies_Problematizing Mobility - a Metaphor of Stickiness, non-places and the kinetic elite.pdf</t>
         </is>
       </c>
       <c r="B126" t="n">
@@ -1698,7 +1698,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Schneider, Bullinger &amp; Brandl_2013_OrgStudies_Resourcing under Tensions.pdf</t>
+          <t>Campbell &amp; van Wanrooy_2013_HR_Long working hours and working-time preferences.pdf</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -1708,7 +1708,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Benschop et al._2013_HR_Discourses of ambition, gender and part time work.pdf</t>
+          <t>Darr &amp; Pinch_2013_OrgStudies_Performing Sales.pdf</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -1718,7 +1718,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Candrian_2013_HR_Taming death and the consequences of discourse.pdf</t>
+          <t>Michaud_2013_OrgStudies_Mediating hte Paradox of Organizational Governance Through Numbers.pdf</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -1728,7 +1728,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Heaphy_2013_OrgSci_Repairing Breaches with Rules Maintaining Institutions.pdf</t>
+          <t>Dhalla &amp; Oliver_2013_OrgStudies_Industry Identity in an Oligopolistic Market and Firms' Responses to Institutional Pressures.pdf</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -1738,7 +1738,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Ashley &amp; Empson_2013_HR_Differentiation and discrimination.pdf</t>
+          <t>Nicholson &amp; Carroll_2013_HR_Identity Undoing and power relations in leadership development.pdf</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -1748,7 +1748,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>McMurray &amp; Ward_2014_Why Would you do that.pdf</t>
+          <t>Whitford &amp; Zirpoli_2014_OrgSci_Pragmatism, Practice, and the Boundaries of Organization.pdf</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -1758,7 +1758,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Meuer_2014_OrgStudies_Archetypes of Inter-firm Relations in the Implementation of Management Innovation.pdf</t>
+          <t>Orr_2014_OrgStudies_Local Government Chief Executive.pdf</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -1768,7 +1768,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Costas &amp; Grey_2014_OrgStudies_The Temporality of Power and the Power of Temporality.pdf</t>
+          <t>Fayard &amp; Metiu_2014_OrgSci_The Role of Writing in Distributed Collaboration.pdf</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -1778,7 +1778,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Tilcsik_2014_ASQ_Imprint-Environment Fit and Performance.pdf</t>
+          <t>Misangyi &amp; Acharya_2014_AMJ_Substitutes or Complements.pdf</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -1788,7 +1788,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Raffaelli &amp; Glynn_2014_AMJ_Turkey or Tailored Relational Pluralism Institutional Complexity and the Organizational Adoption of More or Less Customized PRactices.pdf</t>
+          <t>Tilcsik_2014_ASQ_Imprint-Environment Fit and Performance.pdf</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -1798,7 +1798,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Misangyi &amp; Acharya_2014_AMJ_Substitutes or Complements.pdf</t>
+          <t>Costas &amp; Grey_2014_OrgStudies_The Temporality of Power and the Power of Temporality.pdf</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -1808,7 +1808,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Fayard &amp; Metiu_2014_OrgSci_The Role of Writing in Distributed Collaboration.pdf</t>
+          <t>Meuer_2014_OrgStudies_Archetypes of Inter-firm Relations in the Implementation of Management Innovation.pdf</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -1818,7 +1818,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Orr_2014_OrgStudies_Local Government Chief Executive.pdf</t>
+          <t>McMurray &amp; Ward_2014_Why Would you do that.pdf</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -1828,7 +1828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Whitford &amp; Zirpoli_2014_OrgSci_Pragmatism, Practice, and the Boundaries of Organization.pdf</t>
+          <t>Raffaelli &amp; Glynn_2014_AMJ_Turkey or Tailored Relational Pluralism Institutional Complexity and the Organizational Adoption of More or Less Customized PRactices.pdf</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -1838,7 +1838,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>McCann, Hassart &amp; Granter_2015_HR_Casting the lean spell.pdf</t>
+          <t>Gilmore &amp; Kenny_2015_HR_Work-worlds colliding - self-reflexivity, power and emotion in organizational ethnogrpahy.pdf</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -1848,7 +1848,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Alcadipani, Westowood &amp; Rosa_2015_HR_The politics of identity in organizational ethnographis research.pdf</t>
+          <t>Di Stefano, King &amp; Verona_2015_AMJ_Sanctioning in the Wild Rational Calculus and Retributive Instincts in Gourmet Cuisine.pdf</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -1858,7 +1858,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Mair, Mayer &amp; Lutz_2015_OrgStudies_Navigating Institutional Plurality  - Organizational Governance in Hybrid Organizations.pdf</t>
+          <t>huising_2015_ASQ_To Hive or to Hold Producing Professional Authority through Scut Work.pdf</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -1868,7 +1868,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Riach &amp; Warren_2015_HR_Smell organization - Bodies and corporeal porosity in office work.pdf</t>
+          <t>Hawkins_2015_HR_Ship Shape - Materializing leadership in the British Royal Navy.pdf</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -1878,7 +1878,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Hawkins_2015_HR_Ship Shape - Materializing leadership in the British Royal Navy.pdf</t>
+          <t>Alcadipani, Westowood &amp; Rosa_2015_HR_The politics of identity in organizational ethnographis research.pdf</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -1888,7 +1888,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Gilmore &amp; Kenny_2015_HR_Work-worlds colliding - self-reflexivity, power and emotion in organizational ethnogrpahy.pdf</t>
+          <t>Mair, Mayer &amp; Lutz_2015_OrgStudies_Navigating Institutional Plurality  - Organizational Governance in Hybrid Organizations.pdf</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -1898,7 +1898,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>huising_2015_ASQ_To Hive or to Hold Producing Professional Authority through Scut Work.pdf</t>
+          <t>McCann, Hassart &amp; Granter_2015_HR_Casting the lean spell.pdf</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -1908,7 +1908,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Di Stefano, King &amp; Verona_2015_AMJ_Sanctioning in the Wild Rational Calculus and Retributive Instincts in Gourmet Cuisine.pdf</t>
+          <t>Riach &amp; Warren_2015_HR_Smell organization - Bodies and corporeal porosity in office work.pdf</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -1918,7 +1918,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Pecis_2016_HR_Doing and undoing gender in innovation - feminities and masculinities in innovation proess.pdf</t>
+          <t>Heinze &amp; Weber_2016_OrgSci_Toward Organizational Pluralism.pdf</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -1928,7 +1928,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Fernandez, Marti &amp; Farchi_2016_OrgStudies_Mundane and Everyday Politics for and from the neighbourhood.pdf</t>
+          <t>Aroles &amp; McLean_2016_OrgSci_Rethinking Stability and Change in the Study of Organizational Routines.pdf</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -1938,7 +1938,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Bishop &amp; Waring_2016_HR_Becoming Hybrid.pdf</t>
+          <t>Farias_2016_OrgStudies_Thats what friends are for.pdf</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -1948,7 +1948,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Nelson_2016_OrgSci_How to Share a Really Good Secret.pdf</t>
+          <t>Whitford &amp; Zirpoli_2016_OrgStudies_The Network Firm as a Political Coalition.pdf</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -1958,7 +1958,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Low, Bordia &amp; Bordia_2016_HR_What do Employees want and why.pdf</t>
+          <t>Reedy, King &amp; Coupland_2016_OrgStudies_Organizing for Individuation.pdf</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -1968,7 +1968,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Mavin &amp; Grandy_2016_HR_A Theory of Abject Appearance.pdf</t>
+          <t>Brannan_2016_HR_Power Corruption and Mis-selling.pdf</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -1978,7 +1978,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>O'Toole &amp; Grey_2016_HR_Beyond Choice Thick Volunteering and the Case of the Royal National Lifeboat Institution.pdf</t>
+          <t>Weiss &amp; Huault_2016_OrgStudies_Business as Usual in Financial Markets - The creation of incommensurables as institutional maintenance work.pdf</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -1988,7 +1988,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Nigam et al._2016_ASQ_Explaining the Selection of Routines for Change during Organizational Search.pdf</t>
+          <t>Umney_2016_HR_The Labour Market for Jazz Musicians in Paris and London.pdf</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -1998,7 +1998,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Umney_2016_HR_The Labour Market for Jazz Musicians in Paris and London.pdf</t>
+          <t>Costas &amp; Karreman_2016_HR_The bored self in knowledge work.pdf</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -2008,7 +2008,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Weiss &amp; Huault_2016_OrgStudies_Business as Usual in Financial Markets - The creation of incommensurables as institutional maintenance work.pdf</t>
+          <t>O'Toole &amp; Grey_2016_HR_Beyond Choice Thick Volunteering and the Case of the Royal National Lifeboat Institution.pdf</t>
         </is>
       </c>
       <c r="B158" t="n">
@@ -2018,7 +2018,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Costas &amp; Karreman_2016_HR_The bored self in knowledge work.pdf</t>
+          <t>Mavin &amp; Grandy_2016_HR_A Theory of Abject Appearance.pdf</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -2028,7 +2028,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Brannan_2016_HR_Power Corruption and Mis-selling.pdf</t>
+          <t>Low, Bordia &amp; Bordia_2016_HR_What do Employees want and why.pdf</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -2038,7 +2038,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Reedy, King &amp; Coupland_2016_OrgStudies_Organizing for Individuation.pdf</t>
+          <t>Nelson_2016_OrgSci_How to Share a Really Good Secret.pdf</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -2048,7 +2048,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Whitford &amp; Zirpoli_2016_OrgStudies_The Network Firm as a Political Coalition.pdf</t>
+          <t>Bishop &amp; Waring_2016_HR_Becoming Hybrid.pdf</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -2058,7 +2058,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Farias_2016_OrgStudies_Thats what friends are for.pdf</t>
+          <t>Fernandez, Marti &amp; Farchi_2016_OrgStudies_Mundane and Everyday Politics for and from the neighbourhood.pdf</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -2068,7 +2068,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Aroles &amp; McLean_2016_OrgSci_Rethinking Stability and Change in the Study of Organizational Routines.pdf</t>
+          <t>Pecis_2016_HR_Doing and undoing gender in innovation - feminities and masculinities in innovation proess.pdf</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -2078,7 +2078,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Heinze &amp; Weber_2016_OrgSci_Toward Organizational Pluralism.pdf</t>
+          <t>Nigam et al._2016_ASQ_Explaining the Selection of Routines for Change during Organizational Search.pdf</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -2088,7 +2088,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Handy &amp; Rowlands_2017_HR_The Systems Psychodynamics of Gendered Hiring.pdf</t>
+          <t>Blithe &amp; Wolfe_2017_HR_Work -Life Management in Legal Prostitution.pdf</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -2098,7 +2098,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Pouthier_2017_OrgStudies_Griping and Joking as identificationRituals and Tools for Engagement in Cross-Boundary Team Meetings.pdf</t>
+          <t>Kornberger et al._2017_OrgStudies_When Bureaucracy Meets the Crowd.pdf</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -2108,7 +2108,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Fayard et al._2017_ASQ_How Nascent Occupations Construct a Mandate.pdf</t>
+          <t>Kislov, Hyde &amp; McDonald_2017_OrgStudies_New Game Old Rules - Mechanisms and Consequences of Legitimation in Boundary Spanning Activities.pdf</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -2118,7 +2118,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Ybema &amp; Horvers_2017_OrgStudies_Resistance Through Compliance.pdf</t>
+          <t>Farias_2017_OrgStudies_Money is the root of all evil or is it.pdf</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -2128,7 +2128,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Moisander, Grob &amp; Eraranta_2017_Mechanisms of biopower and neliberal governmentality in precarious work.pdf</t>
+          <t>Gist-Mackey_2017_Disembodied Job Search Communicaiton Training.pdf</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -2138,7 +2138,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Ford et al._2017_OrgStudies_Becoming the Leader - Leadership as a Material Presence.pdf</t>
+          <t>Radoynovska_2017_OrgStudies_Working within Discretionary boundaries.pdf</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -2148,7 +2148,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Visser_2017_J Management Studies _Prying Eyes  A Dramaturgical Approach to Professional Surveillance.pdf</t>
+          <t>Katila et al._2017_AMJ_Is There a Doctor in the House.pdf</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -2158,7 +2158,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Katila et al._2017_AMJ_Is There a Doctor in the House.pdf</t>
+          <t>Moisander, Grob &amp; Eraranta_2017_Mechanisms of biopower and neliberal governmentality in precarious work.pdf</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -2168,7 +2168,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Blithe &amp; Wolfe_2017_HR_Work -Life Management in Legal Prostitution.pdf</t>
+          <t>Ford et al._2017_OrgStudies_Becoming the Leader - Leadership as a Material Presence.pdf</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -2178,7 +2178,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Gist-Mackey_2017_Disembodied Job Search Communicaiton Training.pdf</t>
+          <t>Handy &amp; Rowlands_2017_HR_The Systems Psychodynamics of Gendered Hiring.pdf</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -2188,7 +2188,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Farias_2017_OrgStudies_Money is the root of all evil or is it.pdf</t>
+          <t>Pouthier_2017_OrgStudies_Griping and Joking as identificationRituals and Tools for Engagement in Cross-Boundary Team Meetings.pdf</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -2198,7 +2198,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Kislov, Hyde &amp; McDonald_2017_OrgStudies_New Game Old Rules - Mechanisms and Consequences of Legitimation in Boundary Spanning Activities.pdf</t>
+          <t>Visser_2017_J Management Studies _Prying Eyes  A Dramaturgical Approach to Professional Surveillance.pdf</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -2208,7 +2208,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Kornberger et al._2017_OrgStudies_When Bureaucracy Meets the Crowd.pdf</t>
+          <t>Ybema &amp; Horvers_2017_OrgStudies_Resistance Through Compliance.pdf</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -2218,7 +2218,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Radoynovska_2017_OrgStudies_Working within Discretionary boundaries.pdf</t>
+          <t>Fayard et al._2017_ASQ_How Nascent Occupations Construct a Mandate.pdf</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -2298,7 +2298,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Van Hulst &amp; Ybema_2019_From What to Where.pdf</t>
+          <t>Cohen et al._2019_ASQ_The Role of Accelerator Designs in Mitigating Bounded Rationality in New Ventures.pdf</t>
         </is>
       </c>
       <c r="B187" t="n">
@@ -2308,7 +2308,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Azambula &amp; Islam_2019_HR_Working at the boundaries.pdf</t>
+          <t>Walsh, Pazzaglia &amp; Ergene_2019_HR_Loyal after the End.pdf</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -2318,7 +2318,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Demetry_2019_OrgSci_How Organizations Claim Authenticity The Coproduction of Illusions in Underground Restaurants.pdf</t>
+          <t>Sandholtz, Chung &amp; Waisberg_2019_OrgSci_The Double-Edged Sword of Jurisdictional Entrenchment.pdf</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -2328,7 +2328,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Jack, Riach &amp; Bariola_2019_HR_Temporality and Gendered Agecy.pdf</t>
+          <t>Hales, Riach &amp; Tyler_2019_OrgStudies_Close encounters - intimate service interactions in lap dancing work.pdf</t>
         </is>
       </c>
       <c r="B190" t="n">
@@ -2338,7 +2338,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Guo_2019_HR_Let Our Emotions Tell the Story.pdf</t>
+          <t>Foroughi &amp; Al-Amoudi_2019_OrgStudies_Collective forgetting in a changing organization.pdf</t>
         </is>
       </c>
       <c r="B191" t="n">
@@ -2348,7 +2348,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Vincent &amp; Pagan_2019_HR_Entrepreneurial Agency and Field Relations.pdf</t>
+          <t>Demetry_2019_OrgSci_How Organizations Claim Authenticity The Coproduction of Illusions in Underground Restaurants.pdf</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -2358,7 +2358,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Foroughi &amp; Al-Amoudi_2019_OrgStudies_Collective forgetting in a changing organization.pdf</t>
+          <t>Guo_2019_HR_Let Our Emotions Tell the Story.pdf</t>
         </is>
       </c>
       <c r="B193" t="n">
@@ -2368,7 +2368,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Hales, Riach &amp; Tyler_2019_OrgStudies_Close encounters - intimate service interactions in lap dancing work.pdf</t>
+          <t>Jack, Riach &amp; Bariola_2019_HR_Temporality and Gendered Agecy.pdf</t>
         </is>
       </c>
       <c r="B194" t="n">
@@ -2378,7 +2378,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Sandholtz, Chung &amp; Waisberg_2019_OrgSci_The Double-Edged Sword of Jurisdictional Entrenchment.pdf</t>
+          <t>Azambula &amp; Islam_2019_HR_Working at the boundaries.pdf</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -2388,7 +2388,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Walsh, Pazzaglia &amp; Ergene_2019_HR_Loyal after the End.pdf</t>
+          <t>Vincent &amp; Pagan_2019_HR_Entrepreneurial Agency and Field Relations.pdf</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -2398,7 +2398,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Cohen et al._2019_ASQ_The Role of Accelerator Designs in Mitigating Bounded Rationality in New Ventures.pdf</t>
+          <t>Van Hulst &amp; Ybema_2019_From What to Where.pdf</t>
         </is>
       </c>
       <c r="B197" t="n">
@@ -2408,7 +2408,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Skovgaard-Smith, Soekijad &amp; Down_2020_HR_The Other side of us.pdf</t>
+          <t>DeCelles &amp; Anteby_2020_OrgSci_Compassion in the Clink When and How Human Services Workers Overcome Barriers to Care.pdf</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -2418,7 +2418,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Brown et al._2020_HR_Organizing the Sensory.pdf</t>
+          <t>Hallen, Cohen &amp; Bingham_2020_OrgSci_Do Accelerators Work If So, How.pdf</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -2428,7 +2428,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Kenny, Haugh &amp; Fotaki_2020_HR_Organizational Form and Pro-Social Fantasy in Social Enterprise Creation.pdf</t>
+          <t>Rennstam &amp; Karreman_2020_HR_Understanding control in communities of practice.pdf</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -2438,7 +2438,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Katila, Kuismin &amp; Valtonen_2020_HR_Becoming upbeat.pdf</t>
+          <t>Chliova, Mair &amp; Vernis_2020_OrgStudies_Persistent Category Ambiguity - The case of social entrepreneurship.pdf</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -2448,7 +2448,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>DeCelles &amp; Anteby_2020_OrgSci_Compassion in the Clink When and How Human Services Workers Overcome Barriers to Care.pdf</t>
+          <t>Katila, Kuismin &amp; Valtonen_2020_HR_Becoming upbeat.pdf</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -2458,7 +2458,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Chliova, Mair &amp; Vernis_2020_OrgStudies_Persistent Category Ambiguity - The case of social entrepreneurship.pdf</t>
+          <t>Brown et al._2020_HR_Organizing the Sensory.pdf</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -2468,7 +2468,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Rennstam &amp; Karreman_2020_HR_Understanding control in communities of practice.pdf</t>
+          <t>Skovgaard-Smith, Soekijad &amp; Down_2020_HR_The Other side of us.pdf</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -2478,7 +2478,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Hallen, Cohen &amp; Bingham_2020_OrgSci_Do Accelerators Work If So, How.pdf</t>
+          <t>Kenny, Haugh &amp; Fotaki_2020_HR_Organizational Form and Pro-Social Fantasy in Social Enterprise Creation.pdf</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -2488,7 +2488,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Mikkelsen_2021_HR_Looking over your shoulder.pdf</t>
+          <t>Kozhevnikov_2021_HR_Career Capital in Global Vs Second Order Cities.pdf</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -2498,7 +2498,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Decker, Hassard &amp; Rowlinson_2021_HR_Rethinking History and Memory in Organization Studies.pdf</t>
+          <t>Garcia-Lorenzo, Sell-Trujillo &amp; Donnelly_2021_OrgStudies_Responding to Stigmatization - how to resist and overcome the stigma of unemployment.pdf</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -2508,7 +2508,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Weller, Brown &amp; Clarke_2021_HR_Questing for meaningfulness through narrative identity work.pdf</t>
+          <t>Burchiellaro_2021_OrgStudies_Queering Control and Inclusion the Contemporary Organization.pdf</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -2518,7 +2518,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Zhu &amp; Delbridge_2021_HR_The Management of Second Generation Migrant Workers in China.pdf</t>
+          <t>Brooks, Grgulis &amp; Cook_2021_HR_Unlearning and consent in the UK Fire and Rescue Service.pdf</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -2528,7 +2528,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Ji, Huang &amp; Li_2021_AMJ_Guilt and Corporate Philanthropy The Case of Privatization in China.pdf</t>
+          <t>Morlacchi_2021_OrgStudies_The Performative Power of Frictions and New Possibilities.pdf</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -2538,7 +2538,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Jiang_2021_J Management Studies _The Sharing Economy and Business Model Design  A Configurational Approach.pdf</t>
+          <t>Dawson &amp; Bencherki_2021_HR_Federal Employees or Rogue Rangers.pdf</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -2548,7 +2548,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Morlacchi_2021_OrgStudies_The Performative Power of Frictions and New Possibilities.pdf</t>
+          <t>Ji, Huang &amp; Li_2021_AMJ_Guilt and Corporate Philanthropy The Case of Privatization in China.pdf</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -2558,7 +2558,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Brooks, Grgulis &amp; Cook_2021_HR_Unlearning and consent in the UK Fire and Rescue Service.pdf</t>
+          <t>Zhu &amp; Delbridge_2021_HR_The Management of Second Generation Migrant Workers in China.pdf</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -2568,7 +2568,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Burchiellaro_2021_OrgStudies_Queering Control and Inclusion the Contemporary Organization.pdf</t>
+          <t>Weller, Brown &amp; Clarke_2021_HR_Questing for meaningfulness through narrative identity work.pdf</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -2578,7 +2578,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Dawson &amp; Bencherki_2021_HR_Federal Employees or Rogue Rangers.pdf</t>
+          <t>Decker, Hassard &amp; Rowlinson_2021_HR_Rethinking History and Memory in Organization Studies.pdf</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -2588,7 +2588,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Garcia-Lorenzo, Sell-Trujillo &amp; Donnelly_2021_OrgStudies_Responding to Stigmatization - how to resist and overcome the stigma of unemployment.pdf</t>
+          <t>Mikkelsen_2021_HR_Looking over your shoulder.pdf</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -2598,7 +2598,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Kozhevnikov_2021_HR_Career Capital in Global Vs Second Order Cities.pdf</t>
+          <t>Jiang_2021_J Management Studies _The Sharing Economy and Business Model Design  A Configurational Approach.pdf</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -2608,7 +2608,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Bharatan, Swan &amp; Oborn_2022_HR_NAvigating Turbulent waters.pdf</t>
+          <t>Villeseche, Meloui &amp; Jha_2022_HR_Feminism in Women's Business Networks.pdf</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -2618,7 +2618,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Baikovich, Wasserman &amp; Pfefferman_2022_OrgStudies_Evolution from the inside out - revisiting hte impact of reproductive resistance among ultra orthodox female entrepreneurs.pdf</t>
+          <t>Payne &amp; Butler_2022_HR_Of Charities and Choice.pdf</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -2628,7 +2628,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Mikkelsen_2022_HR_Looking over your shoulder.pdf</t>
+          <t>Cioce, Korczynski &amp; Pero_2022_HR_The improvised language of solidarity.pdf</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -2638,7 +2638,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Toubiana &amp; Ruebottom_2022_Stigma Hierarchies - The Internal Dynamics of Stigmatization in the Sex Work Occupation.pdf</t>
+          <t>Marsh &amp; Sliwa_2022_OrgStudies_Making a difference through atmospheres.pdf</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -2648,7 +2648,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Stanko et al., _2022_OrgStudies_Navigating an Identity Playground - using sociomateriality to build a theory of identity play.pdf</t>
+          <t>Mikkelsen_2022_HR_Looking over your shoulder.pdf</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -2658,7 +2658,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Marsh &amp; Sliwa_2022_OrgStudies_Making a difference through atmospheres.pdf</t>
+          <t>Toubiana &amp; Ruebottom_2022_Stigma Hierarchies - The Internal Dynamics of Stigmatization in the Sex Work Occupation.pdf</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -2668,7 +2668,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Cioce, Korczynski &amp; Pero_2022_HR_The improvised language of solidarity.pdf</t>
+          <t>Baikovich, Wasserman &amp; Pfefferman_2022_OrgStudies_Evolution from the inside out - revisiting hte impact of reproductive resistance among ultra orthodox female entrepreneurs.pdf</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -2678,7 +2678,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Payne &amp; Butler_2022_HR_Of Charities and Choice.pdf</t>
+          <t>Bharatan, Swan &amp; Oborn_2022_HR_NAvigating Turbulent waters.pdf</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -2688,7 +2688,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Villeseche, Meloui &amp; Jha_2022_HR_Feminism in Women's Business Networks.pdf</t>
+          <t>Cameron_2022_OrgSci_Making Out While Driving - Relational and Efficiency Games in the Gig Economy.pdf</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -2698,7 +2698,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Cameron_2022_OrgSci_Making Out While Driving - Relational and Efficiency Games in the Gig Economy.pdf</t>
+          <t>Stanko et al., _2022_OrgStudies_Navigating an Identity Playground - using sociomateriality to build a theory of identity play.pdf</t>
         </is>
       </c>
       <c r="B227" t="n">

</xml_diff>

<commit_message>
ocr updates - gotta catch em all
</commit_message>
<xml_diff>
--- a/no_extracted_figure_papers.xlsx
+++ b/no_extracted_figure_papers.xlsx
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
+          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Salk &amp; Shenkar_2001_OrgSci_Social Identities in an Int JV.pdf</t>
+          <t>Offerman &amp; Spiros_2001_AMJ_The Science and Practice of team Development Improving the Link.pdf</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
+          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,7 +588,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Labianca et al._2001_OrgSci_Emulation in Academia_Quant.pdf</t>
+          <t>Amabile et al._AMJ_2001_Academic Practitioner Collaboration in Management Research.pdf</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -678,7 +678,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sorge &amp; Brussig_2003_OrgSci_Organizational Process, Strategic Content and Socio-Economic Resources.pdf</t>
+          <t>Bechky_2003_OrgSci_Sharing Meaning across Occupational Communities.pdf</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -698,7 +698,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bechky_2003_OrgSci_Sharing Meaning across Occupational Communities.pdf</t>
+          <t>Sorge &amp; Brussig_2003_OrgSci_Organizational Process, Strategic Content and Socio-Economic Resources.pdf</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -738,7 +738,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Hardy_2003_J Management Studies _ Resources  Knowledge and Influence  The Organizational Effects of Interorganizational.pdf</t>
+          <t>Piderit_2003_J Management Studies - Breaking Silence  Tactical Choices Women Managers Make in Speaking Up About.pdf</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -748,7 +748,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Piderit_2003_J Management Studies - Breaking Silence  Tactical Choices Women Managers Make in Speaking Up About.pdf</t>
+          <t>Hardy_2003_J Management Studies _ Resources  Knowledge and Influence  The Organizational Effects of Interorganizational.pdf</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -768,7 +768,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Banerjee &amp; Linstead_2004_HR_Masking subversion.pdf</t>
+          <t>El-Sawad, Arnold &amp; Cohen_2004_HR_Doublethink the prevalence and function of contradiction in accounts of org life.pdf</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -778,7 +778,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical and linguistic moves for a moving display.pdf</t>
+          <t>Graebner &amp; Eisenhardt_2004_ASQ_The Seller's Side of the Story - Acquisiation as Courtship and Governance as Syndicate.pdf</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -788,7 +788,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical linguistic moves.pdf</t>
+          <t>Procter &amp; Currie_2004_HR_Target based teamworking - groups work and interdependence in the UK Civil Service.pdf</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,7 +798,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>El-Sawad, Arnold &amp; Cohen_2004_HR_Doublethink the prevalence and function of contradiction in accounts of org life.pdf</t>
+          <t>Banerjee &amp; Linstead_2004_HR_Masking subversion.pdf</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -808,7 +808,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Graebner &amp; Eisenhardt_2004_ASQ_The Seller's Side of the Story - Acquisiation as Courtship and Governance as Syndicate.pdf</t>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical and linguistic moves for a moving display.pdf</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -818,7 +818,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Procter &amp; Currie_2004_HR_Target based teamworking - groups work and interdependence in the UK Civil Service.pdf</t>
+          <t>Samra-Fredericks_2004_HR_Managerial elites making rhetorical linguistic moves.pdf</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -828,7 +828,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Collin-Jacques &amp; Smith_2004_HR_Nursing on the line - Experiences from England and Quebec.pdf</t>
+          <t>Evans et al._2004_ASQ_Beach Time Bridge Time and Billable Hours.pdf</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -838,7 +838,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Hoegl et al_2004_OrgSci_Interteam Coordination Project Commitment and Teamwork.pdf</t>
+          <t>Cross &amp; Sproull_2004_OrgSci_More Than an Answer - Information Relationships for Actionable Knowledge.pdf</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -848,7 +848,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Clegg_2004_J Management Studies _ Political Hybrids  Tocquevillean Views on Project Organizations.pdf</t>
+          <t>Maguire, Hardy &amp; Lawrence_2004_AMJ_Institutional Entrepreneurship in Emerging Fields HIV AIDS Treatment Advocacy in Canada.pdf</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -858,7 +858,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Evans et al._2004_ASQ_Beach Time Bridge Time and Billable Hours.pdf</t>
+          <t>Collin-Jacques &amp; Smith_2004_HR_Nursing on the line - Experiences from England and Quebec.pdf</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -868,7 +868,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Cross &amp; Sproull_2004_OrgSci_More Than an Answer - Information Relationships for Actionable Knowledge.pdf</t>
+          <t>Hoegl et al_2004_OrgSci_Interteam Coordination Project Commitment and Teamwork.pdf</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -878,7 +878,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Maguire, Hardy &amp; Lawrence_2004_AMJ_Institutional Entrepreneurship in Emerging Fields HIV AIDS Treatment Advocacy in Canada.pdf</t>
+          <t>Clegg_2004_J Management Studies _ Political Hybrids  Tocquevillean Views on Project Organizations.pdf</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -888,7 +888,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Perkins_2005_J Management Studies _ Ordering Top Pay  Interpreting the Signals.pdf</t>
+          <t>Whittle_2005_HR_Preaching and practising flexibility.pdf</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -898,7 +898,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Whittle_2005_HR_Preaching and practising flexibility.pdf</t>
+          <t>Suddaby &amp; Greenwod_2005_ASQ_Rhetorical Strategies of Legitimacy_Content Analysis.pdf</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Suddaby &amp; Greenwod_2005_ASQ_Rhetorical Strategies of Legitimacy_Content Analysis.pdf</t>
+          <t>D'Abate_2005_HR_Working hard or hardly working - a study of individuals engaging in personal business ont he job.pdf</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,7 +918,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>D'Abate_2005_HR_Working hard or hardly working - a study of individuals engaging in personal business ont he job.pdf</t>
+          <t>Perkins_2005_J Management Studies _ Ordering Top Pay  Interpreting the Signals.pdf</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ferlie et al._2005_AMJ_The Nonspread of Innovations The Mediating Role of Professionals.pdf</t>
+          <t>Goltz_2005_HR_Women's appeals for equity at American universities.pdf</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,7 +958,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Dowd &amp; Kaplan_2005_HR_The career life of academics - boundaried or boundaryless.pdf</t>
+          <t>Ferlie et al._2005_AMJ_The Nonspread of Innovations The Mediating Role of Professionals.pdf</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -968,7 +968,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Arndt &amp; Bigelow_2005_ASQ_Professionalizing and Masculanizing a Female Occupation_Archival.pdf</t>
+          <t>Dowd &amp; Kaplan_2005_HR_The career life of academics - boundaried or boundaryless.pdf</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -978,7 +978,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Goltz_2005_HR_Women's appeals for equity at American universities.pdf</t>
+          <t>Arndt &amp; Bigelow_2005_ASQ_Professionalizing and Masculanizing a Female Occupation_Archival.pdf</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -1248,7 +1248,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
+          <t>Berg, Grant &amp; Johnson_2010_OrgSci_When Callings Are Calling Crafting Work and Leisure in Pursuit of Unanswered Occupational Callings.pdf</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -1258,7 +1258,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Berg, Grant &amp; Johnson_2010_OrgSci_When Callings Are Calling Crafting Work and Leisure in Pursuit of Unanswered Occupational Callings.pdf</t>
+          <t>Detert &amp; Trevino_2010_OrgSci_Speaking Up to Higher-Ups.pdf</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1268,7 +1268,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Detert &amp; Trevino_2010_OrgSci_Speaking Up to Higher-Ups.pdf</t>
+          <t>Finn, Currie &amp; Martin_2010_OrgStudies_Team Work in Context - Institutional Mediation in the Public-service Professional Bureaucracy.pdf</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1318,7 +1318,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Finn, Currie &amp; Martin_2010_OrgStudies_Team Work in Context - Institutional Mediation in the Public-service Professional Bureaucracy.pdf</t>
+          <t>Azoulay et al._2010_ASQ_Nasty Brutish and Short - Embeddedness Failure in the Pharma Industry.pdf</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1368,7 +1368,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
+          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -1378,7 +1378,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
+          <t>Clark et al._2010_ASQ_Transitional Identity as a Facilitator of Organizational Identity Change during a Merger.pdf</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -1388,7 +1388,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
+          <t>Tilcsik_2010_AMJ_From Ritual to Reality.pdf</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1398,7 +1398,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Cabantous, Gond &amp; Johnson -Cramer_2010_OrgStudies_Decision Theory as PRactice - Crafting Rationality in Organizations.pdf</t>
+          <t>Gioia et al_2010_ASQ_Forging an Identity.pdf</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -1408,7 +1408,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Walsh &amp; Bartuken_2011_AMJ_Cheating the Fates Organizational Foundings in the Wake of Demise.pdf</t>
+          <t>Fiss_2011_AMJ_Building Better Causal Theories.pdf</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -1418,7 +1418,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Fiss_2011_AMJ_Building Better Causal Theories.pdf</t>
+          <t>Walsh &amp; Bartuken_2011_AMJ_Cheating the Fates Organizational Foundings in the Wake of Demise.pdf</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -1448,7 +1448,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Greckhamer_2011_OrgStudies_Cross-cultural Differences in Compensation Level and Inequality across Occupations.pdf</t>
+          <t>Matusik &amp; Mickel_2011_HR_Embracing or embattled by converged mobile devices.pdf</t>
         </is>
       </c>
       <c r="B102" t="n">
@@ -1458,7 +1458,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Matusik &amp; Mickel_2011_HR_Embracing or embattled by converged mobile devices.pdf</t>
+          <t>Greckhamer_2011_OrgStudies_Cross-cultural Differences in Compensation Level and Inequality across Occupations.pdf</t>
         </is>
       </c>
       <c r="B103" t="n">
@@ -1468,7 +1468,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Crowley_2012_OrgStudies_Control and Dignity in Professional, Manual and Service-Sector Employment.pdf</t>
+          <t>Browning &amp; McNamee_2012_HR_Considering the temporary leader in temporary work arrangements.pdf</t>
         </is>
       </c>
       <c r="B104" t="n">
@@ -1478,7 +1478,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Willems et al._2012_HR_Volunteer decisions not to leave - reasons to quit versus functional motivates to stay.pdf</t>
+          <t>Wright, Nyberg &amp; Grant_2012_OrgStudies_Hippies on the third floor - climage change, narrative identity and the micro-politics of corporate environmentalism.pdf</t>
         </is>
       </c>
       <c r="B105" t="n">
@@ -1488,7 +1488,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Currie &amp; White_2012_OrgStudies_Inter-professional Barriers and Knowledge Brokering in an Organizational Context.pdf</t>
+          <t>Grugulis &amp; Stoyanova_2012_OrgStudies_Social Capital and Networks in Film and TV.pdf</t>
         </is>
       </c>
       <c r="B106" t="n">
@@ -1498,7 +1498,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Browning &amp; McNamee_2012_HR_Considering the temporary leader in temporary work arrangements.pdf</t>
+          <t>Crowley_2012_OrgStudies_Control and Dignity in Professional, Manual and Service-Sector Employment.pdf</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1508,7 +1508,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Wright, Nyberg &amp; Grant_2012_OrgStudies_Hippies on the third floor - climage change, narrative identity and the micro-politics of corporate environmentalism.pdf</t>
+          <t>Willems et al._2012_HR_Volunteer decisions not to leave - reasons to quit versus functional motivates to stay.pdf</t>
         </is>
       </c>
       <c r="B108" t="n">
@@ -1518,7 +1518,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Grugulis &amp; Stoyanova_2012_OrgStudies_Social Capital and Networks in Film and TV.pdf</t>
+          <t>Currie &amp; White_2012_OrgStudies_Inter-professional Barriers and Knowledge Brokering in an Organizational Context.pdf</t>
         </is>
       </c>
       <c r="B109" t="n">
@@ -1548,7 +1548,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Kenny_2012_OrgStudies_Somoene Big and Important.pdf</t>
+          <t>McCann_2012_J Management Studies_Still Blue‐Collar after all these Years  An Ethnography of the Professionalization.pdf</t>
         </is>
       </c>
       <c r="B112" t="n">
@@ -1558,7 +1558,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Willis_2012_HR_Witnesses on the periphery.pdf</t>
+          <t>Mork &amp; Hoholm_2012_HR_Changing practice through boundary organizing.pdf</t>
         </is>
       </c>
       <c r="B113" t="n">
@@ -1568,7 +1568,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Rennstam_2012_OrgStudies_Object Control a Study of Technologically Dense Knowledge Work.pdf</t>
+          <t>Watson &amp; Watson_2012_HR_Narratives in Society.pdf</t>
         </is>
       </c>
       <c r="B114" t="n">
@@ -1588,7 +1588,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>McCann_2012_J Management Studies_Still Blue‐Collar after all these Years  An Ethnography of the Professionalization.pdf</t>
+          <t>Kenny_2012_OrgStudies_Somoene Big and Important.pdf</t>
         </is>
       </c>
       <c r="B116" t="n">
@@ -1598,7 +1598,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Mork &amp; Hoholm_2012_HR_Changing practice through boundary organizing.pdf</t>
+          <t>Willis_2012_HR_Witnesses on the periphery.pdf</t>
         </is>
       </c>
       <c r="B117" t="n">
@@ -1608,7 +1608,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Watson &amp; Watson_2012_HR_Narratives in Society.pdf</t>
+          <t>Rennstam_2012_OrgStudies_Object Control a Study of Technologically Dense Knowledge Work.pdf</t>
         </is>
       </c>
       <c r="B118" t="n">
@@ -1618,7 +1618,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Ashley &amp; Empson_2013_HR_Differentiation and discrimination.pdf</t>
+          <t>Michaud_2013_OrgStudies_Mediating hte Paradox of Organizational Governance Through Numbers.pdf</t>
         </is>
       </c>
       <c r="B119" t="n">
@@ -1628,7 +1628,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Heaphy_2013_OrgSci_Repairing Breaches with Rules Maintaining Institutions.pdf</t>
+          <t>Darr &amp; Pinch_2013_OrgStudies_Performing Sales.pdf</t>
         </is>
       </c>
       <c r="B120" t="n">
@@ -1638,7 +1638,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Candrian_2013_HR_Taming death and the consequences of discourse.pdf</t>
+          <t>McPherson &amp; Sauder_2013_ASQ_Logics in Action - Managing Institutional Complexity in Drug Court.pdf</t>
         </is>
       </c>
       <c r="B121" t="n">
@@ -1668,7 +1668,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>McPherson &amp; Sauder_2013_ASQ_Logics in Action - Managing Institutional Complexity in Drug Court.pdf</t>
+          <t>Dhalla &amp; Oliver_2013_OrgStudies_Industry Identity in an Oligopolistic Market and Firms' Responses to Institutional Pressures.pdf</t>
         </is>
       </c>
       <c r="B124" t="n">
@@ -1678,7 +1678,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Benschop et al._2013_HR_Discourses of ambition, gender and part time work.pdf</t>
+          <t>Ashley &amp; Empson_2013_HR_Differentiation and discrimination.pdf</t>
         </is>
       </c>
       <c r="B125" t="n">
@@ -1708,7 +1708,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Darr &amp; Pinch_2013_OrgStudies_Performing Sales.pdf</t>
+          <t>Nicholson &amp; Carroll_2013_HR_Identity Undoing and power relations in leadership development.pdf</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -1718,7 +1718,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Michaud_2013_OrgStudies_Mediating hte Paradox of Organizational Governance Through Numbers.pdf</t>
+          <t>Benschop et al._2013_HR_Discourses of ambition, gender and part time work.pdf</t>
         </is>
       </c>
       <c r="B129" t="n">
@@ -1728,7 +1728,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Dhalla &amp; Oliver_2013_OrgStudies_Industry Identity in an Oligopolistic Market and Firms' Responses to Institutional Pressures.pdf</t>
+          <t>Candrian_2013_HR_Taming death and the consequences of discourse.pdf</t>
         </is>
       </c>
       <c r="B130" t="n">
@@ -1738,7 +1738,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Nicholson &amp; Carroll_2013_HR_Identity Undoing and power relations in leadership development.pdf</t>
+          <t>Heaphy_2013_OrgSci_Repairing Breaches with Rules Maintaining Institutions.pdf</t>
         </is>
       </c>
       <c r="B131" t="n">
@@ -1748,7 +1748,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Whitford &amp; Zirpoli_2014_OrgSci_Pragmatism, Practice, and the Boundaries of Organization.pdf</t>
+          <t>Meuer_2014_OrgStudies_Archetypes of Inter-firm Relations in the Implementation of Management Innovation.pdf</t>
         </is>
       </c>
       <c r="B132" t="n">
@@ -1758,7 +1758,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Orr_2014_OrgStudies_Local Government Chief Executive.pdf</t>
+          <t>Costas &amp; Grey_2014_OrgStudies_The Temporality of Power and the Power of Temporality.pdf</t>
         </is>
       </c>
       <c r="B133" t="n">
@@ -1768,7 +1768,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Fayard &amp; Metiu_2014_OrgSci_The Role of Writing in Distributed Collaboration.pdf</t>
+          <t>Tilcsik_2014_ASQ_Imprint-Environment Fit and Performance.pdf</t>
         </is>
       </c>
       <c r="B134" t="n">
@@ -1778,7 +1778,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Misangyi &amp; Acharya_2014_AMJ_Substitutes or Complements.pdf</t>
+          <t>Whitford &amp; Zirpoli_2014_OrgSci_Pragmatism, Practice, and the Boundaries of Organization.pdf</t>
         </is>
       </c>
       <c r="B135" t="n">
@@ -1788,7 +1788,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Tilcsik_2014_ASQ_Imprint-Environment Fit and Performance.pdf</t>
+          <t>McMurray &amp; Ward_2014_Why Would you do that.pdf</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -1798,7 +1798,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Costas &amp; Grey_2014_OrgStudies_The Temporality of Power and the Power of Temporality.pdf</t>
+          <t>Raffaelli &amp; Glynn_2014_AMJ_Turkey or Tailored Relational Pluralism Institutional Complexity and the Organizational Adoption of More or Less Customized PRactices.pdf</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -1808,7 +1808,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Meuer_2014_OrgStudies_Archetypes of Inter-firm Relations in the Implementation of Management Innovation.pdf</t>
+          <t>Misangyi &amp; Acharya_2014_AMJ_Substitutes or Complements.pdf</t>
         </is>
       </c>
       <c r="B138" t="n">
@@ -1818,7 +1818,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>McMurray &amp; Ward_2014_Why Would you do that.pdf</t>
+          <t>Fayard &amp; Metiu_2014_OrgSci_The Role of Writing in Distributed Collaboration.pdf</t>
         </is>
       </c>
       <c r="B139" t="n">
@@ -1828,7 +1828,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Raffaelli &amp; Glynn_2014_AMJ_Turkey or Tailored Relational Pluralism Institutional Complexity and the Organizational Adoption of More or Less Customized PRactices.pdf</t>
+          <t>Orr_2014_OrgStudies_Local Government Chief Executive.pdf</t>
         </is>
       </c>
       <c r="B140" t="n">
@@ -1838,7 +1838,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Gilmore &amp; Kenny_2015_HR_Work-worlds colliding - self-reflexivity, power and emotion in organizational ethnogrpahy.pdf</t>
+          <t>huising_2015_ASQ_To Hive or to Hold Producing Professional Authority through Scut Work.pdf</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -1848,7 +1848,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Di Stefano, King &amp; Verona_2015_AMJ_Sanctioning in the Wild Rational Calculus and Retributive Instincts in Gourmet Cuisine.pdf</t>
+          <t>Hawkins_2015_HR_Ship Shape - Materializing leadership in the British Royal Navy.pdf</t>
         </is>
       </c>
       <c r="B142" t="n">
@@ -1858,7 +1858,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>huising_2015_ASQ_To Hive or to Hold Producing Professional Authority through Scut Work.pdf</t>
+          <t>Gilmore &amp; Kenny_2015_HR_Work-worlds colliding - self-reflexivity, power and emotion in organizational ethnogrpahy.pdf</t>
         </is>
       </c>
       <c r="B143" t="n">
@@ -1868,7 +1868,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Hawkins_2015_HR_Ship Shape - Materializing leadership in the British Royal Navy.pdf</t>
+          <t>Di Stefano, King &amp; Verona_2015_AMJ_Sanctioning in the Wild Rational Calculus and Retributive Instincts in Gourmet Cuisine.pdf</t>
         </is>
       </c>
       <c r="B144" t="n">
@@ -1878,7 +1878,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Alcadipani, Westowood &amp; Rosa_2015_HR_The politics of identity in organizational ethnographis research.pdf</t>
+          <t>Riach &amp; Warren_2015_HR_Smell organization - Bodies and corporeal porosity in office work.pdf</t>
         </is>
       </c>
       <c r="B145" t="n">
@@ -1888,7 +1888,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Mair, Mayer &amp; Lutz_2015_OrgStudies_Navigating Institutional Plurality  - Organizational Governance in Hybrid Organizations.pdf</t>
+          <t>McCann, Hassart &amp; Granter_2015_HR_Casting the lean spell.pdf</t>
         </is>
       </c>
       <c r="B146" t="n">
@@ -1898,7 +1898,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>McCann, Hassart &amp; Granter_2015_HR_Casting the lean spell.pdf</t>
+          <t>Mair, Mayer &amp; Lutz_2015_OrgStudies_Navigating Institutional Plurality  - Organizational Governance in Hybrid Organizations.pdf</t>
         </is>
       </c>
       <c r="B147" t="n">
@@ -1908,7 +1908,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Riach &amp; Warren_2015_HR_Smell organization - Bodies and corporeal porosity in office work.pdf</t>
+          <t>Alcadipani, Westowood &amp; Rosa_2015_HR_The politics of identity in organizational ethnographis research.pdf</t>
         </is>
       </c>
       <c r="B148" t="n">
@@ -1918,7 +1918,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Heinze &amp; Weber_2016_OrgSci_Toward Organizational Pluralism.pdf</t>
+          <t>Low, Bordia &amp; Bordia_2016_HR_What do Employees want and why.pdf</t>
         </is>
       </c>
       <c r="B149" t="n">
@@ -1928,7 +1928,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Aroles &amp; McLean_2016_OrgSci_Rethinking Stability and Change in the Study of Organizational Routines.pdf</t>
+          <t>Mavin &amp; Grandy_2016_HR_A Theory of Abject Appearance.pdf</t>
         </is>
       </c>
       <c r="B150" t="n">
@@ -1938,7 +1938,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Farias_2016_OrgStudies_Thats what friends are for.pdf</t>
+          <t>Umney_2016_HR_The Labour Market for Jazz Musicians in Paris and London.pdf</t>
         </is>
       </c>
       <c r="B151" t="n">
@@ -1948,7 +1948,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Whitford &amp; Zirpoli_2016_OrgStudies_The Network Firm as a Political Coalition.pdf</t>
+          <t>Heinze &amp; Weber_2016_OrgSci_Toward Organizational Pluralism.pdf</t>
         </is>
       </c>
       <c r="B152" t="n">
@@ -1958,7 +1958,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Reedy, King &amp; Coupland_2016_OrgStudies_Organizing for Individuation.pdf</t>
+          <t>Aroles &amp; McLean_2016_OrgSci_Rethinking Stability and Change in the Study of Organizational Routines.pdf</t>
         </is>
       </c>
       <c r="B153" t="n">
@@ -1968,7 +1968,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Brannan_2016_HR_Power Corruption and Mis-selling.pdf</t>
+          <t>Farias_2016_OrgStudies_Thats what friends are for.pdf</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -1988,7 +1988,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Umney_2016_HR_The Labour Market for Jazz Musicians in Paris and London.pdf</t>
+          <t>Nelson_2016_OrgSci_How to Share a Really Good Secret.pdf</t>
         </is>
       </c>
       <c r="B156" t="n">
@@ -1998,7 +1998,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Costas &amp; Karreman_2016_HR_The bored self in knowledge work.pdf</t>
+          <t>Whitford &amp; Zirpoli_2016_OrgStudies_The Network Firm as a Political Coalition.pdf</t>
         </is>
       </c>
       <c r="B157" t="n">
@@ -2018,7 +2018,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Mavin &amp; Grandy_2016_HR_A Theory of Abject Appearance.pdf</t>
+          <t>Bishop &amp; Waring_2016_HR_Becoming Hybrid.pdf</t>
         </is>
       </c>
       <c r="B159" t="n">
@@ -2028,7 +2028,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Low, Bordia &amp; Bordia_2016_HR_What do Employees want and why.pdf</t>
+          <t>Fernandez, Marti &amp; Farchi_2016_OrgStudies_Mundane and Everyday Politics for and from the neighbourhood.pdf</t>
         </is>
       </c>
       <c r="B160" t="n">
@@ -2038,7 +2038,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Nelson_2016_OrgSci_How to Share a Really Good Secret.pdf</t>
+          <t>Pecis_2016_HR_Doing and undoing gender in innovation - feminities and masculinities in innovation proess.pdf</t>
         </is>
       </c>
       <c r="B161" t="n">
@@ -2048,7 +2048,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Bishop &amp; Waring_2016_HR_Becoming Hybrid.pdf</t>
+          <t>Nigam et al._2016_ASQ_Explaining the Selection of Routines for Change during Organizational Search.pdf</t>
         </is>
       </c>
       <c r="B162" t="n">
@@ -2058,7 +2058,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Fernandez, Marti &amp; Farchi_2016_OrgStudies_Mundane and Everyday Politics for and from the neighbourhood.pdf</t>
+          <t>Costas &amp; Karreman_2016_HR_The bored self in knowledge work.pdf</t>
         </is>
       </c>
       <c r="B163" t="n">
@@ -2068,7 +2068,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Pecis_2016_HR_Doing and undoing gender in innovation - feminities and masculinities in innovation proess.pdf</t>
+          <t>Brannan_2016_HR_Power Corruption and Mis-selling.pdf</t>
         </is>
       </c>
       <c r="B164" t="n">
@@ -2078,7 +2078,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Nigam et al._2016_ASQ_Explaining the Selection of Routines for Change during Organizational Search.pdf</t>
+          <t>Reedy, King &amp; Coupland_2016_OrgStudies_Organizing for Individuation.pdf</t>
         </is>
       </c>
       <c r="B165" t="n">
@@ -2088,7 +2088,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Blithe &amp; Wolfe_2017_HR_Work -Life Management in Legal Prostitution.pdf</t>
+          <t>Katila et al._2017_AMJ_Is There a Doctor in the House.pdf</t>
         </is>
       </c>
       <c r="B166" t="n">
@@ -2098,7 +2098,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Kornberger et al._2017_OrgStudies_When Bureaucracy Meets the Crowd.pdf</t>
+          <t>Farias_2017_OrgStudies_Money is the root of all evil or is it.pdf</t>
         </is>
       </c>
       <c r="B167" t="n">
@@ -2108,7 +2108,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Kislov, Hyde &amp; McDonald_2017_OrgStudies_New Game Old Rules - Mechanisms and Consequences of Legitimation in Boundary Spanning Activities.pdf</t>
+          <t>Blithe &amp; Wolfe_2017_HR_Work -Life Management in Legal Prostitution.pdf</t>
         </is>
       </c>
       <c r="B168" t="n">
@@ -2118,7 +2118,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Farias_2017_OrgStudies_Money is the root of all evil or is it.pdf</t>
+          <t>Kornberger et al._2017_OrgStudies_When Bureaucracy Meets the Crowd.pdf</t>
         </is>
       </c>
       <c r="B169" t="n">
@@ -2128,7 +2128,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Gist-Mackey_2017_Disembodied Job Search Communicaiton Training.pdf</t>
+          <t>Kislov, Hyde &amp; McDonald_2017_OrgStudies_New Game Old Rules - Mechanisms and Consequences of Legitimation in Boundary Spanning Activities.pdf</t>
         </is>
       </c>
       <c r="B170" t="n">
@@ -2138,7 +2138,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Radoynovska_2017_OrgStudies_Working within Discretionary boundaries.pdf</t>
+          <t>Gist-Mackey_2017_Disembodied Job Search Communicaiton Training.pdf</t>
         </is>
       </c>
       <c r="B171" t="n">
@@ -2148,7 +2148,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Katila et al._2017_AMJ_Is There a Doctor in the House.pdf</t>
+          <t>Radoynovska_2017_OrgStudies_Working within Discretionary boundaries.pdf</t>
         </is>
       </c>
       <c r="B172" t="n">
@@ -2158,7 +2158,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Moisander, Grob &amp; Eraranta_2017_Mechanisms of biopower and neliberal governmentality in precarious work.pdf</t>
+          <t>Fayard et al._2017_ASQ_How Nascent Occupations Construct a Mandate.pdf</t>
         </is>
       </c>
       <c r="B173" t="n">
@@ -2168,7 +2168,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Ford et al._2017_OrgStudies_Becoming the Leader - Leadership as a Material Presence.pdf</t>
+          <t>Moisander, Grob &amp; Eraranta_2017_Mechanisms of biopower and neliberal governmentality in precarious work.pdf</t>
         </is>
       </c>
       <c r="B174" t="n">
@@ -2178,7 +2178,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Handy &amp; Rowlands_2017_HR_The Systems Psychodynamics of Gendered Hiring.pdf</t>
+          <t>Visser_2017_J Management Studies _Prying Eyes  A Dramaturgical Approach to Professional Surveillance.pdf</t>
         </is>
       </c>
       <c r="B175" t="n">
@@ -2188,7 +2188,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Pouthier_2017_OrgStudies_Griping and Joking as identificationRituals and Tools for Engagement in Cross-Boundary Team Meetings.pdf</t>
+          <t>Ybema &amp; Horvers_2017_OrgStudies_Resistance Through Compliance.pdf</t>
         </is>
       </c>
       <c r="B176" t="n">
@@ -2198,7 +2198,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Visser_2017_J Management Studies _Prying Eyes  A Dramaturgical Approach to Professional Surveillance.pdf</t>
+          <t>Ford et al._2017_OrgStudies_Becoming the Leader - Leadership as a Material Presence.pdf</t>
         </is>
       </c>
       <c r="B177" t="n">
@@ -2208,7 +2208,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Ybema &amp; Horvers_2017_OrgStudies_Resistance Through Compliance.pdf</t>
+          <t>Pouthier_2017_OrgStudies_Griping and Joking as identificationRituals and Tools for Engagement in Cross-Boundary Team Meetings.pdf</t>
         </is>
       </c>
       <c r="B178" t="n">
@@ -2218,7 +2218,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Fayard et al._2017_ASQ_How Nascent Occupations Construct a Mandate.pdf</t>
+          <t>Handy &amp; Rowlands_2017_HR_The Systems Psychodynamics of Gendered Hiring.pdf</t>
         </is>
       </c>
       <c r="B179" t="n">
@@ -2308,7 +2308,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Walsh, Pazzaglia &amp; Ergene_2019_HR_Loyal after the End.pdf</t>
+          <t>Vincent &amp; Pagan_2019_HR_Entrepreneurial Agency and Field Relations.pdf</t>
         </is>
       </c>
       <c r="B188" t="n">
@@ -2318,7 +2318,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Sandholtz, Chung &amp; Waisberg_2019_OrgSci_The Double-Edged Sword of Jurisdictional Entrenchment.pdf</t>
+          <t>Azambula &amp; Islam_2019_HR_Working at the boundaries.pdf</t>
         </is>
       </c>
       <c r="B189" t="n">
@@ -2348,7 +2348,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Demetry_2019_OrgSci_How Organizations Claim Authenticity The Coproduction of Illusions in Underground Restaurants.pdf</t>
+          <t>Sandholtz, Chung &amp; Waisberg_2019_OrgSci_The Double-Edged Sword of Jurisdictional Entrenchment.pdf</t>
         </is>
       </c>
       <c r="B192" t="n">
@@ -2378,7 +2378,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Azambula &amp; Islam_2019_HR_Working at the boundaries.pdf</t>
+          <t>Walsh, Pazzaglia &amp; Ergene_2019_HR_Loyal after the End.pdf</t>
         </is>
       </c>
       <c r="B195" t="n">
@@ -2388,7 +2388,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Vincent &amp; Pagan_2019_HR_Entrepreneurial Agency and Field Relations.pdf</t>
+          <t>Demetry_2019_OrgSci_How Organizations Claim Authenticity The Coproduction of Illusions in Underground Restaurants.pdf</t>
         </is>
       </c>
       <c r="B196" t="n">
@@ -2408,7 +2408,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>DeCelles &amp; Anteby_2020_OrgSci_Compassion in the Clink When and How Human Services Workers Overcome Barriers to Care.pdf</t>
+          <t>Rennstam &amp; Karreman_2020_HR_Understanding control in communities of practice.pdf</t>
         </is>
       </c>
       <c r="B198" t="n">
@@ -2418,7 +2418,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Hallen, Cohen &amp; Bingham_2020_OrgSci_Do Accelerators Work If So, How.pdf</t>
+          <t>Chliova, Mair &amp; Vernis_2020_OrgStudies_Persistent Category Ambiguity - The case of social entrepreneurship.pdf</t>
         </is>
       </c>
       <c r="B199" t="n">
@@ -2428,7 +2428,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Rennstam &amp; Karreman_2020_HR_Understanding control in communities of practice.pdf</t>
+          <t>Hallen, Cohen &amp; Bingham_2020_OrgSci_Do Accelerators Work If So, How.pdf</t>
         </is>
       </c>
       <c r="B200" t="n">
@@ -2438,7 +2438,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Chliova, Mair &amp; Vernis_2020_OrgStudies_Persistent Category Ambiguity - The case of social entrepreneurship.pdf</t>
+          <t>DeCelles &amp; Anteby_2020_OrgSci_Compassion in the Clink When and How Human Services Workers Overcome Barriers to Care.pdf</t>
         </is>
       </c>
       <c r="B201" t="n">
@@ -2448,7 +2448,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Katila, Kuismin &amp; Valtonen_2020_HR_Becoming upbeat.pdf</t>
+          <t>Skovgaard-Smith, Soekijad &amp; Down_2020_HR_The Other side of us.pdf</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -2458,7 +2458,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Brown et al._2020_HR_Organizing the Sensory.pdf</t>
+          <t>Katila, Kuismin &amp; Valtonen_2020_HR_Becoming upbeat.pdf</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -2468,7 +2468,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Skovgaard-Smith, Soekijad &amp; Down_2020_HR_The Other side of us.pdf</t>
+          <t>Kenny, Haugh &amp; Fotaki_2020_HR_Organizational Form and Pro-Social Fantasy in Social Enterprise Creation.pdf</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -2478,7 +2478,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Kenny, Haugh &amp; Fotaki_2020_HR_Organizational Form and Pro-Social Fantasy in Social Enterprise Creation.pdf</t>
+          <t>Brown et al._2020_HR_Organizing the Sensory.pdf</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -2608,7 +2608,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Villeseche, Meloui &amp; Jha_2022_HR_Feminism in Women's Business Networks.pdf</t>
+          <t>Payne &amp; Butler_2022_HR_Of Charities and Choice.pdf</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -2618,7 +2618,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Payne &amp; Butler_2022_HR_Of Charities and Choice.pdf</t>
+          <t>Cioce, Korczynski &amp; Pero_2022_HR_The improvised language of solidarity.pdf</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -2628,7 +2628,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Cioce, Korczynski &amp; Pero_2022_HR_The improvised language of solidarity.pdf</t>
+          <t>Stanko et al., _2022_OrgStudies_Navigating an Identity Playground - using sociomateriality to build a theory of identity play.pdf</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -2648,7 +2648,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Mikkelsen_2022_HR_Looking over your shoulder.pdf</t>
+          <t>Cameron_2022_OrgSci_Making Out While Driving - Relational and Efficiency Games in the Gig Economy.pdf</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -2668,7 +2668,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Baikovich, Wasserman &amp; Pfefferman_2022_OrgStudies_Evolution from the inside out - revisiting hte impact of reproductive resistance among ultra orthodox female entrepreneurs.pdf</t>
+          <t>Mikkelsen_2022_HR_Looking over your shoulder.pdf</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -2678,7 +2678,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Bharatan, Swan &amp; Oborn_2022_HR_NAvigating Turbulent waters.pdf</t>
+          <t>Baikovich, Wasserman &amp; Pfefferman_2022_OrgStudies_Evolution from the inside out - revisiting hte impact of reproductive resistance among ultra orthodox female entrepreneurs.pdf</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -2688,7 +2688,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Cameron_2022_OrgSci_Making Out While Driving - Relational and Efficiency Games in the Gig Economy.pdf</t>
+          <t>Bharatan, Swan &amp; Oborn_2022_HR_NAvigating Turbulent waters.pdf</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -2698,7 +2698,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Stanko et al., _2022_OrgStudies_Navigating an Identity Playground - using sociomateriality to build a theory of identity play.pdf</t>
+          <t>Villeseche, Meloui &amp; Jha_2022_HR_Feminism in Women's Business Networks.pdf</t>
         </is>
       </c>
       <c r="B227" t="n">

</xml_diff>